<commit_message>
version 1 révisée pour A2024
</commit_message>
<xml_diff>
--- a/template/grille_correction.xlsx
+++ b/template/grille_correction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/developpementweb3/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notescours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A0B4D8-AF2E-EB4B-A1FA-3B8B98D7FFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED954C9-00B7-B546-9465-A394C2234997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
   <si>
     <t>Élément</t>
   </si>
@@ -153,15 +153,6 @@
     <t>L’interface applicative n’implémente pas correctement de méthodes GET avec transformations, ou ces requêtes ne sont pas pertinentes au projet</t>
   </si>
   <si>
-    <t xml:space="preserve">L’interface applicative implémente correctement un minimum de 2 propriétés virtuelles (ou l’équivalent). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’interface applicative n'implémente pas correctement un minimum de 2 propriétés virtuelles (ou l’équivalent). </t>
-  </si>
-  <si>
-    <t>Propriétés virtuelles</t>
-  </si>
-  <si>
     <t>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.</t>
   </si>
   <si>
@@ -238,9 +229,6 @@
   </si>
   <si>
     <t>La documentation de l’interface applicative est floue ou incomplète.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’interface applicative implémente correctement une propriété virtuelle (ou l’équivalent). </t>
   </si>
   <si>
     <t>__Application Web (50%)__ {: colspan=5}</t>
@@ -440,9 +428,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -480,7 +468,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -586,7 +574,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -728,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -736,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>IF(LEN(modèle!A2) &gt; 0, modèle!A2,"")</f>
         <v>__Base de données (10%)__ {: colspan=5}</v>
@@ -798,7 +786,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>IF(LEN(modèle!A3) &gt; 0, modèle!A3,"")</f>
         <v>Choix</v>
@@ -824,7 +812,7 @@
         <v>Le choix du SGBD n’est pas du tout approprié.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>IF(LEN(modèle!A4) &gt; 0, modèle!A4,"")</f>
         <v>Schéma</v>
@@ -876,7 +864,7 @@
         <v>La base de données n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>IF(LEN(modèle!A6) &gt; 0, modèle!A6,"")</f>
         <v>Jeu de tests</v>
@@ -928,7 +916,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>IF(LEN(modèle!A8) &gt; 0, modèle!A8,"")</f>
         <v>Méthodes HTTP</v>
@@ -954,7 +942,7 @@
         <v>L’interface applicative implémente __moins de 25%__ des méthodes HTTP demandées. &lt;br/&gt; (GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(LEN(modèle!A9) &gt; 0, modèle!A9,"")</f>
         <v>GET avec filtre</v>
@@ -980,7 +968,7 @@
         <v>L’interface applicative n’implémente pas correctement de méthodes GET avec filtres, ou ces requêtes ne sont pas pertinentes au projet&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(LEN(modèle!A10) &gt; 0, modèle!A10,"")</f>
         <v>GET avec transformation</v>
@@ -1006,14 +994,14 @@
         <v>L’interface applicative n’implémente pas correctement de méthodes GET avec transformations, ou ces requêtes ne sont pas pertinentes au projet&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>IF(LEN(modèle!A11) &gt; 0, modèle!A11,"")</f>
-        <v>Propriétés virtuelles</v>
+        <v>Validations natives</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B11) &gt; 0, modèle!B11,""),IF(LEN(modèle!C11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C11,IF(modèle!C11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente correctement un minimum de 2 propriétés virtuelles (ou l’équivalent). &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D11) &gt; 0, modèle!D11,""),IF(LEN(modèle!E11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E11,IF(modèle!E11 &gt; 1," points"," point")),""))</f>
@@ -1021,7 +1009,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F11) &gt; 0, modèle!F11,""),IF(LEN(modèle!G11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G11,IF(modèle!G11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente correctement une propriété virtuelle (ou l’équivalent). &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>L’interface applicative contient des __validations natives__ partiellement appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H11) &gt; 0, modèle!H11,""),IF(LEN(modèle!I11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I11,IF(modèle!I11 &gt; 1," points"," point")),""))</f>
@@ -1029,17 +1017,17 @@
       </c>
       <c r="F11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J11) &gt; 0, modèle!J11,""),IF(LEN(modèle!K11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K11,IF(modèle!K11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n'implémente pas correctement un minimum de 2 propriétés virtuelles (ou l’équivalent). &lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’interface applicative ne contient pas de __validations natives__ appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(LEN(modèle!A12) &gt; 0, modèle!A12,"")</f>
-        <v>Validations natives</v>
+        <v>Validations personnalisées</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B12) &gt; 0, modèle!B12,""),IF(LEN(modèle!C12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C12,IF(modèle!C12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative contient au minimum 2 __validations personnalisées__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D12) &gt; 0, modèle!D12,""),IF(LEN(modèle!E12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E12,IF(modèle!E12 &gt; 1," points"," point")),""))</f>
@@ -1047,7 +1035,7 @@
       </c>
       <c r="D12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F12) &gt; 0, modèle!F12,""),IF(LEN(modèle!G12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G12,IF(modèle!G12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des __validations natives__ partiellement appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative contient au moins 1 __validation personnalisée__ appropriée aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H12) &gt; 0, modèle!H12,""),IF(LEN(modèle!I12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I12,IF(modèle!I12 &gt; 1," points"," point")),""))</f>
@@ -1055,17 +1043,17 @@
       </c>
       <c r="F12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J12) &gt; 0, modèle!J12,""),IF(LEN(modèle!K12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K12,IF(modèle!K12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de __validations natives__ appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’interface applicative ne contient pas de __validation personnalisée__ appropriée aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>IF(LEN(modèle!A13) &gt; 0, modèle!A13,"")</f>
-        <v>Validations personnalisées</v>
+        <v>Application sécurisée</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B13) &gt; 0, modèle!B13,""),IF(LEN(modèle!C13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C13,IF(modèle!C13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient au minimum 2 __validations personnalisées__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;6 points</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D13) &gt; 0, modèle!D13,""),IF(LEN(modèle!E13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E13,IF(modèle!E13 &gt; 1," points"," point")),""))</f>
@@ -1073,7 +1061,7 @@
       </c>
       <c r="D13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F13) &gt; 0, modèle!F13,""),IF(LEN(modèle!G13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G13,IF(modèle!G13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient au moins 1 __validation personnalisée__ appropriée aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H13) &gt; 0, modèle!H13,""),IF(LEN(modèle!I13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I13,IF(modèle!I13 &gt; 1," points"," point")),""))</f>
@@ -1081,17 +1069,17 @@
       </c>
       <c r="F13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J13) &gt; 0, modèle!J13,""),IF(LEN(modèle!K13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K13,IF(modèle!K13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de __validation personnalisée__ appropriée aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’interface applicative n’est pas __sécurisée__.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>IF(LEN(modèle!A14) &gt; 0, modèle!A14,"")</f>
-        <v>Application sécurisée</v>
+        <v>Messages d'erreur</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B14) &gt; 0, modèle!B14,""),IF(LEN(modèle!C14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C14,IF(modèle!C14 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D14) &gt; 0, modèle!D14,""),IF(LEN(modèle!E14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E14,IF(modèle!E14 &gt; 1," points"," point")),""))</f>
@@ -1099,7 +1087,7 @@
       </c>
       <c r="D14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F14) &gt; 0, modèle!F14,""),IF(LEN(modèle!G14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G14,IF(modèle!G14 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H14) &gt; 0, modèle!H14,""),IF(LEN(modèle!I14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I14,IF(modèle!I14 &gt; 1," points"," point")),""))</f>
@@ -1107,17 +1095,17 @@
       </c>
       <c r="F14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J14) &gt; 0, modèle!J14,""),IF(LEN(modèle!K14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K14,IF(modèle!K14 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas __sécurisée__.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’interface applicative ne contient pas de messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>IF(LEN(modèle!A15) &gt; 0, modèle!A15,"")</f>
-        <v>Messages d'erreur</v>
+        <v>Publication</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B15) &gt; 0, modèle!B15,""),IF(LEN(modèle!C15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C15,IF(modèle!C15 &gt; 1," points"," point")),""))</f>
-        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative est publiée et fonctionnelle. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D15) &gt; 0, modèle!D15,""),IF(LEN(modèle!E15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E15,IF(modèle!E15 &gt; 1," points"," point")),""))</f>
@@ -1125,7 +1113,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F15) &gt; 0, modèle!F15,""),IF(LEN(modèle!G15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G15,IF(modèle!G15 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative n’est pas correctement publiée. &lt;br/&gt;Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H15) &gt; 0, modèle!H15,""),IF(LEN(modèle!I15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I15,IF(modèle!I15 &gt; 1," points"," point")),""))</f>
@@ -1133,17 +1121,17 @@
       </c>
       <c r="F15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J15) &gt; 0, modèle!J15,""),IF(LEN(modèle!K15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K15,IF(modèle!K15 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’interface applicative n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f>IF(LEN(modèle!A16) &gt; 0, modèle!A16,"")</f>
-        <v>Publication</v>
+        <v>Documentation</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B16) &gt; 0, modèle!B16,""),IF(LEN(modèle!C16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C16,IF(modèle!C16 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est publiée et fonctionnelle. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D16) &gt; 0, modèle!D16,""),IF(LEN(modèle!E16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E16,IF(modèle!E16 &gt; 1," points"," point")),""))</f>
@@ -1151,7 +1139,7 @@
       </c>
       <c r="D16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F16) &gt; 0, modèle!F16,""),IF(LEN(modèle!G16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G16,IF(modèle!G16 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée. &lt;br/&gt;Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H16) &gt; 0, modèle!H16,""),IF(LEN(modèle!I16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I16,IF(modèle!I16 &gt; 1," points"," point")),""))</f>
@@ -1159,17 +1147,17 @@
       </c>
       <c r="F16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J16) &gt; 0, modèle!J16,""),IF(LEN(modèle!K16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K16,IF(modèle!K16 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>IF(LEN(modèle!A17) &gt; 0, modèle!A17,"")</f>
-        <v>Documentation</v>
+        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B17) &gt; 0, modèle!B17,""),IF(LEN(modèle!C17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C17,IF(modèle!C17 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D17) &gt; 0, modèle!D17,""),IF(LEN(modèle!E17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E17,IF(modèle!E17 &gt; 1," points"," point")),""))</f>
@@ -1177,7 +1165,7 @@
       </c>
       <c r="D17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F17) &gt; 0, modèle!F17,""),IF(LEN(modèle!G17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G17,IF(modèle!G17 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="E17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H17) &gt; 0, modèle!H17,""),IF(LEN(modèle!I17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I17,IF(modèle!I17 &gt; 1," points"," point")),""))</f>
@@ -1185,13 +1173,13 @@
       </c>
       <c r="F17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J17) &gt; 0, modèle!J17,""),IF(LEN(modèle!K17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K17,IF(modèle!K17 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(LEN(modèle!A18) &gt; 0, modèle!A18,"")</f>
-        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
+        <v>__Application Web (50%)__ {: colspan=5}</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B18) &gt; 0, modèle!B18,""),IF(LEN(modèle!C18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C18,IF(modèle!C18 &gt; 1," points"," point")),""))</f>
@@ -1214,14 +1202,14 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(LEN(modèle!A19) &gt; 0, modèle!A19,"")</f>
-        <v>__Application Web (50%)__ {: colspan=5}</v>
+        <v>Composants</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B19) &gt; 0, modèle!B19,""),IF(LEN(modèle!C19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C19,IF(modèle!C19 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D19) &gt; 0, modèle!D19,""),IF(LEN(modèle!E19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E19,IF(modèle!E19 &gt; 1," points"," point")),""))</f>
@@ -1229,103 +1217,103 @@
       </c>
       <c r="D19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F19) &gt; 0, modèle!F19,""),IF(LEN(modèle!G19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G19,IF(modèle!G19 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H19) &gt; 0, modèle!H19,""),IF(LEN(modèle!I19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I19,IF(modèle!I19 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J19) &gt; 0, modèle!J19,""),IF(LEN(modèle!K19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K19,IF(modèle!K19 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(LEN(modèle!A20) &gt; 0, modèle!A20,"")</f>
-        <v>Composants</v>
+        <v>Hooks</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B20) &gt; 0, modèle!B20,""),IF(LEN(modèle!C20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C20,IF(modèle!C20 &gt; 1," points"," point")),""))</f>
-        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D20) &gt; 0, modèle!D20,""),IF(LEN(modèle!E20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E20,IF(modèle!E20 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F20) &gt; 0, modèle!F20,""),IF(LEN(modèle!G20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G20,IF(modèle!G20 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H20) &gt; 0, modèle!H20,""),IF(LEN(modèle!I20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I20,IF(modèle!I20 &gt; 1," points"," point")),""))</f>
-        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="F20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J20) &gt; 0, modèle!J20,""),IF(LEN(modèle!K20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K20,IF(modèle!K20 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(LEN(modèle!A21) &gt; 0, modèle!A21,"")</f>
-        <v>Hooks</v>
+        <v>Méthodes HTTP</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B21) &gt; 0, modèle!B21,""),IF(LEN(modèle!C21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C21,IF(modèle!C21 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D21) &gt; 0, modèle!D21,""),IF(LEN(modèle!E21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E21,IF(modèle!E21 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
       </c>
       <c r="D21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F21) &gt; 0, modèle!F21,""),IF(LEN(modèle!G21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G21,IF(modèle!G21 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H21) &gt; 0, modèle!H21,""),IF(LEN(modèle!I21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I21,IF(modèle!I21 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="F21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J21) &gt; 0, modèle!J21,""),IF(LEN(modèle!K21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K21,IF(modèle!K21 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f>IF(LEN(modèle!A22) &gt; 0, modèle!A22,"")</f>
-        <v>Méthodes HTTP</v>
+        <v>Validations</v>
       </c>
       <c r="B22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B22) &gt; 0, modèle!B22,""),IF(LEN(modèle!C22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C22,IF(modèle!C22 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
+        <v>L’application contient des validations appropriées.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D22) &gt; 0, modèle!D22,""),IF(LEN(modèle!E22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E22,IF(modèle!E22 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
+        <v/>
       </c>
       <c r="D22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F22) &gt; 0, modèle!F22,""),IF(LEN(modèle!G22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G22,IF(modèle!G22 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
+        <v>L’application contient des validations partiellement appropriées.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H22) &gt; 0, modèle!H22,""),IF(LEN(modèle!I22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I22,IF(modèle!I22 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="F22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J22) &gt; 0, modèle!J22,""),IF(LEN(modèle!K22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K22,IF(modèle!K22 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application ne contient pas de validations appropriées.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>IF(LEN(modèle!A23) &gt; 0, modèle!A23,"")</f>
-        <v>Validations</v>
+        <v>Visuel</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B23) &gt; 0, modèle!B23,""),IF(LEN(modèle!C23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C23,IF(modèle!C23 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations appropriées.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D23) &gt; 0, modèle!D23,""),IF(LEN(modèle!E23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E23,IF(modèle!E23 &gt; 1," points"," point")),""))</f>
@@ -1333,7 +1321,7 @@
       </c>
       <c r="D23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F23) &gt; 0, modèle!F23,""),IF(LEN(modèle!G23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G23,IF(modèle!G23 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations partiellement appropriées.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H23) &gt; 0, modèle!H23,""),IF(LEN(modèle!I23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I23,IF(modèle!I23 &gt; 1," points"," point")),""))</f>
@@ -1341,17 +1329,17 @@
       </c>
       <c r="F23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J23) &gt; 0, modèle!J23,""),IF(LEN(modèle!K23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K23,IF(modèle!K23 &gt; 1," points"," point")),""))</f>
-        <v>L’application ne contient pas de validations appropriées.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f>IF(LEN(modèle!A24) &gt; 0, modèle!A24,"")</f>
-        <v>Visuel</v>
+        <v>Application sécurisée</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B24) &gt; 0, modèle!B24,""),IF(LEN(modèle!C24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C24,IF(modèle!C24 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D24) &gt; 0, modèle!D24,""),IF(LEN(modèle!E24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E24,IF(modèle!E24 &gt; 1," points"," point")),""))</f>
@@ -1359,7 +1347,7 @@
       </c>
       <c r="D24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F24) &gt; 0, modèle!F24,""),IF(LEN(modèle!G24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G24,IF(modèle!G24 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H24) &gt; 0, modèle!H24,""),IF(LEN(modèle!I24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I24,IF(modèle!I24 &gt; 1," points"," point")),""))</f>
@@ -1367,17 +1355,17 @@
       </c>
       <c r="F24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J24) &gt; 0, modèle!J24,""),IF(LEN(modèle!K24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K24,IF(modèle!K24 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f>IF(LEN(modèle!A25) &gt; 0, modèle!A25,"")</f>
-        <v>Application sécurisée</v>
+        <v>Internationalisation</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B25) &gt; 0, modèle!B25,""),IF(LEN(modèle!C25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C25,IF(modèle!C25 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’application est entièrement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D25) &gt; 0, modèle!D25,""),IF(LEN(modèle!E25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E25,IF(modèle!E25 &gt; 1," points"," point")),""))</f>
@@ -1385,7 +1373,7 @@
       </c>
       <c r="D25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F25) &gt; 0, modèle!F25,""),IF(LEN(modèle!G25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G25,IF(modèle!G25 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est partiellement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H25) &gt; 0, modèle!H25,""),IF(LEN(modèle!I25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I25,IF(modèle!I25 &gt; 1," points"," point")),""))</f>
@@ -1393,17 +1381,17 @@
       </c>
       <c r="F25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J25) &gt; 0, modèle!J25,""),IF(LEN(modèle!K25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K25,IF(modèle!K25 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f>IF(LEN(modèle!A26) &gt; 0, modèle!A26,"")</f>
-        <v>Internationalisation</v>
+        <v>Organisation visuelle</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B26) &gt; 0, modèle!B26,""),IF(LEN(modèle!C26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C26,IF(modèle!C26 &gt; 1," points"," point")),""))</f>
-        <v>L’application est entièrement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D26) &gt; 0, modèle!D26,""),IF(LEN(modèle!E26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E26,IF(modèle!E26 &gt; 1," points"," point")),""))</f>
@@ -1411,7 +1399,7 @@
       </c>
       <c r="D26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F26) &gt; 0, modèle!F26,""),IF(LEN(modèle!G26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G26,IF(modèle!G26 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H26) &gt; 0, modèle!H26,""),IF(LEN(modèle!I26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I26,IF(modèle!I26 &gt; 1," points"," point")),""))</f>
@@ -1419,17 +1407,17 @@
       </c>
       <c r="F26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J26) &gt; 0, modèle!J26,""),IF(LEN(modèle!K26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K26,IF(modèle!K26 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
         <f>IF(LEN(modèle!A27) &gt; 0, modèle!A27,"")</f>
-        <v>Organisation visuelle</v>
+        <v>Navigation</v>
       </c>
       <c r="B27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B27) &gt; 0, modèle!B27,""),IF(LEN(modèle!C27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C27,IF(modèle!C27 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D27) &gt; 0, modèle!D27,""),IF(LEN(modèle!E27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E27,IF(modèle!E27 &gt; 1," points"," point")),""))</f>
@@ -1437,7 +1425,7 @@
       </c>
       <c r="D27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F27) &gt; 0, modèle!F27,""),IF(LEN(modèle!G27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G27,IF(modèle!G27 &gt; 1," points"," point")),""))</f>
-        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H27) &gt; 0, modèle!H27,""),IF(LEN(modèle!I27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I27,IF(modèle!I27 &gt; 1," points"," point")),""))</f>
@@ -1445,17 +1433,17 @@
       </c>
       <c r="F27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J27) &gt; 0, modèle!J27,""),IF(LEN(modèle!K27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K27,IF(modèle!K27 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
         <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
-        <v>Navigation</v>
+        <v>PWA</v>
       </c>
       <c r="B28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
-        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 75% des exigences.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
@@ -1463,7 +1451,7 @@
       </c>
       <c r="D28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
-        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 50% des exigences.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
@@ -1471,17 +1459,17 @@
       </c>
       <c r="F28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
-        <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application est configurée en tant qu’application progressive (PWA) ou répond à moins de 50% des exigences.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="str">
         <f>IF(LEN(modèle!A29) &gt; 0, modèle!A29,"")</f>
-        <v>PWA</v>
+        <v>Publication</v>
       </c>
       <c r="B29" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B29) &gt; 0, modèle!B29,""),IF(LEN(modèle!C29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C29,IF(modèle!C29 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 75% des exigences.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C29" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D29) &gt; 0, modèle!D29,""),IF(LEN(modèle!E29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E29,IF(modèle!E29 &gt; 1," points"," point")),""))</f>
@@ -1489,7 +1477,7 @@
       </c>
       <c r="D29" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F29) &gt; 0, modèle!F29,""),IF(LEN(modèle!G29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G29,IF(modèle!G29 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 50% des exigences.&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E29" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H29) &gt; 0, modèle!H29,""),IF(LEN(modèle!I29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I29,IF(modèle!I29 &gt; 1," points"," point")),""))</f>
@@ -1497,17 +1485,17 @@
       </c>
       <c r="F29" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J29) &gt; 0, modèle!J29,""),IF(LEN(modèle!K29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K29,IF(modèle!K29 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) ou répond à moins de 50% des exigences.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="str">
         <f>IF(LEN(modèle!A30) &gt; 0, modèle!A30,"")</f>
-        <v>Publication</v>
+        <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B30" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B30) &gt; 0, modèle!B30,""),IF(LEN(modèle!C30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C30,IF(modèle!C30 &gt; 1," points"," point")),""))</f>
-        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="C30" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D30) &gt; 0, modèle!D30,""),IF(LEN(modèle!E30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E30,IF(modèle!E30 &gt; 1," points"," point")),""))</f>
@@ -1515,7 +1503,7 @@
       </c>
       <c r="D30" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F30) &gt; 0, modèle!F30,""),IF(LEN(modèle!G30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G30,IF(modèle!G30 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v/>
       </c>
       <c r="E30" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H30) &gt; 0, modèle!H30,""),IF(LEN(modèle!I30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I30,IF(modèle!I30 &gt; 1," points"," point")),""))</f>
@@ -1523,32 +1511,6 @@
       </c>
       <c r="F30" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J30) &gt; 0, modèle!J30,""),IF(LEN(modèle!K30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K30,IF(modèle!K30 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="str">
-        <f>IF(LEN(modèle!A31) &gt; 0, modèle!A31,"")</f>
-        <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
-      </c>
-      <c r="B31" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B31) &gt; 0, modèle!B31,""),IF(LEN(modèle!C31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C31,IF(modèle!C31 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="C31" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D31) &gt; 0, modèle!D31,""),IF(LEN(modèle!E31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E31,IF(modèle!E31 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="D31" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F31) &gt; 0, modèle!F31,""),IF(LEN(modèle!G31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G31,IF(modèle!G31 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="E31" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H31) &gt; 0, modèle!H31,""),IF(LEN(modèle!I31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I31,IF(modèle!I31 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="F31" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J31) &gt; 0, modèle!J31,""),IF(LEN(modèle!K31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K31,IF(modèle!K31 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
@@ -1559,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004F3CC3-38A6-1349-9E0D-D575CD7A9164}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,7 +1564,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1661,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M29" si="0">MAX(C4,E4,G4,I4)</f>
+        <f t="shared" ref="M4:M20" si="0">MAX(C4,E4,G4,I4)</f>
         <v>4</v>
       </c>
     </row>
@@ -1715,7 +1677,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
@@ -1827,51 +1789,51 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
       <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1883,19 +1845,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>47</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" t="s">
         <v>48</v>
@@ -1905,27 +1867,27 @@
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1937,19 +1899,19 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J15" t="s">
         <v>56</v>
@@ -1959,24 +1921,24 @@
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
       <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16">
         <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
       </c>
       <c r="J16" t="s">
         <v>59</v>
@@ -1986,38 +1948,20 @@
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>62</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>64</v>
       </c>
       <c r="M18">
@@ -2027,37 +1971,61 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
         <v>68</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20">
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2069,79 +2037,73 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21">
         <v>3</v>
       </c>
-      <c r="F21" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
       <c r="J21" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" ref="M21:M29" si="1">MAX(C21,E21,G21,I21)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
         <v>76</v>
       </c>
       <c r="G22">
-        <v>7</v>
-      </c>
-      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" t="s">
         <v>77</v>
       </c>
-      <c r="I22">
-        <v>3</v>
-      </c>
-      <c r="J22" t="s">
-        <v>78</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22:M31" si="1">MAX(C22,E22,G22,I22)</f>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>79</v>
@@ -2150,13 +2112,13 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -2166,75 +2128,75 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
         <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>85</v>
       </c>
       <c r="G24">
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" t="s">
         <v>87</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>88</v>
       </c>
       <c r="G25">
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
       </c>
       <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>91</v>
+        <v>3</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" t="s">
         <v>92</v>
@@ -2244,39 +2206,39 @@
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
         <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="J27" t="s">
-        <v>96</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
         <v>97</v>
@@ -2285,13 +2247,13 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2303,7 +2265,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>101</v>
@@ -2312,13 +2274,13 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2328,36 +2290,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>107</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>108</v>
+    <row r="30" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changement de domaine + projet intégrateur
</commit_message>
<xml_diff>
--- a/template/grille_correction.xlsx
+++ b/template/grille_correction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notescours/developpementweb3/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED954C9-00B7-B546-9465-A394C2234997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7D37F-B90C-D441-802F-464E4783595F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Élément</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Insuffisant</t>
   </si>
   <si>
-    <t>Choix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le choix du SGBD est pertinent. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le choix du SGBD n’est pas optimal. </t>
-  </si>
-  <si>
-    <t>Le choix du SGBD n’est pas du tout approprié.</t>
-  </si>
-  <si>
     <t>Schéma</t>
   </si>
   <si>
@@ -108,21 +96,6 @@
     <t>Méthodes HTTP</t>
   </si>
   <si>
-    <t>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)</t>
-  </si>
-  <si>
-    <t>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)</t>
-  </si>
-  <si>
-    <t>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)</t>
-  </si>
-  <si>
-    <t>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)</t>
-  </si>
-  <si>
-    <t>L’interface applicative implémente __moins de 25%__ des méthodes HTTP demandées. &lt;br/&gt; (GET, POST, PUT, PATCH, DELETE)</t>
-  </si>
-  <si>
     <t xml:space="preserve">L’interface applicative implémente correctement un minimum de 2 méthodes GET avec filtres. Ces requêtes sont pertinentes au projet.  </t>
   </si>
   <si>
@@ -138,21 +111,6 @@
     <t>GET avec filtre</t>
   </si>
   <si>
-    <t>GET avec transformation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’interface applicative implémente correctement un minimum de 2 méthodes GET avec transformations. Ces requêtes sont pertinentes au projet.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’interface applicative implémente partiellement un minimum de 2 méthodes GET avec transformations. Ces requêtes sont pertinentes au projet.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’interface applicative implémente partiellement moins de 2 méthodes GET avec transformations. Ces requêtes sont peu pertinentes au projet.  </t>
-  </si>
-  <si>
-    <t>L’interface applicative n’implémente pas correctement de méthodes GET avec transformations, ou ces requêtes ne sont pas pertinentes au projet</t>
-  </si>
-  <si>
     <t>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.</t>
   </si>
   <si>
@@ -264,15 +222,6 @@
     <t>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).</t>
   </si>
   <si>
-    <t>L’application contient des validations appropriées.</t>
-  </si>
-  <si>
-    <t>L’application contient des validations partiellement appropriées.</t>
-  </si>
-  <si>
-    <t>L’application ne contient pas de validations appropriées.</t>
-  </si>
-  <si>
     <t>Validations</t>
   </si>
   <si>
@@ -297,15 +246,6 @@
     <t>L’application n’est pas sécurisée.</t>
   </si>
   <si>
-    <t>L’application est entièrement internationalisée dans un minimum de 2 langues</t>
-  </si>
-  <si>
-    <t>L’application est partiellement internationalisée dans un minimum de 2 langues</t>
-  </si>
-  <si>
-    <t>L’application n’est pas internationalisée dans un minimum de 2 langues</t>
-  </si>
-  <si>
     <t>Internationalisation</t>
   </si>
   <si>
@@ -370,6 +310,39 @@
   </si>
   <si>
     <t>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks</t>
+  </si>
+  <si>
+    <t>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)</t>
+  </si>
+  <si>
+    <t>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, DELETE)</t>
+  </si>
+  <si>
+    <t>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)</t>
+  </si>
+  <si>
+    <t>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)</t>
+  </si>
+  <si>
+    <t>L’interface applicative implémente __moins de 25%__ des méthodes HTTP demandées. &lt;br/&gt; (GET, POST, PUT, DELETE)</t>
+  </si>
+  <si>
+    <t>L’application est partiellement internationaliséeen Français et en Anglais</t>
+  </si>
+  <si>
+    <t>L’application n’est pas internationalisée en Français et en Anglais</t>
+  </si>
+  <si>
+    <t>L’application contient des validations appropriées avec messages à l'utilisateur dans l'interface graphique.</t>
+  </si>
+  <si>
+    <t>L’application contient des validations partiellement appropriées qui ont des messages affichés à l'utilisateur.</t>
+  </si>
+  <si>
+    <t>L’application ne contient pas de validations appropriées ou ne sont pas affichées à l'utilisateur.</t>
+  </si>
+  <si>
+    <t>L’application est entièrement internationalisée en Français et en Anglais</t>
   </si>
 </sst>
 </file>
@@ -724,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,48 +759,48 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>IF(LEN(modèle!A3) &gt; 0, modèle!A3,"")</f>
-        <v>Choix</v>
+        <v>Schéma</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B3) &gt; 0, modèle!B3,""),IF(LEN(modèle!C3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C3,IF(modèle!C3 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Le schéma de la base de données répond totalement aux exigences demandées. &lt;br/&gt;&lt;br/&gt;6 points</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D3) &gt; 0, modèle!D3,""),IF(LEN(modèle!E3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E3,IF(modèle!E3 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Un ou 2 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F3) &gt; 0, modèle!F3,""),IF(LEN(modèle!G3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G3,IF(modèle!G3 &gt; 1," points"," point")),""))</f>
-        <v>Le choix du SGBD est pertinent. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>3 à 5 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H3) &gt; 0, modèle!H3,""),IF(LEN(modèle!I3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I3,IF(modèle!I3 &gt; 1," points"," point")),""))</f>
-        <v>Le choix du SGBD n’est pas optimal. &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v/>
       </c>
       <c r="F3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J3) &gt; 0, modèle!J3,""),IF(LEN(modèle!K3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K3,IF(modèle!K3 &gt; 1," points"," point")),""))</f>
-        <v>Le choix du SGBD n’est pas du tout approprié.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>Plus de 5 éléments ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>IF(LEN(modèle!A4) &gt; 0, modèle!A4,"")</f>
-        <v>Schéma</v>
+        <v>Publication</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B4) &gt; 0, modèle!B4,""),IF(LEN(modèle!C4) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C4,IF(modèle!C4 &gt; 1," points"," point")),""))</f>
-        <v>Le schéma de la base de données répond totalement aux exigences demandées. &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D4) &gt; 0, modèle!D4,""),IF(LEN(modèle!E4) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E4,IF(modèle!E4 &gt; 1," points"," point")),""))</f>
-        <v>Un ou 2 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="D4" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F4) &gt; 0, modèle!F4,""),IF(LEN(modèle!G4) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G4,IF(modèle!G4 &gt; 1," points"," point")),""))</f>
-        <v>3 à 5 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>Le base de données est publiée. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H4) &gt; 0, modèle!H4,""),IF(LEN(modèle!I4) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I4,IF(modèle!I4 &gt; 1," points"," point")),""))</f>
@@ -835,17 +808,17 @@
       </c>
       <c r="F4" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J4) &gt; 0, modèle!J4,""),IF(LEN(modèle!K4) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K4,IF(modèle!K4 &gt; 1," points"," point")),""))</f>
-        <v>Plus de 5 éléments ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>La base de données n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>IF(LEN(modèle!A5) &gt; 0, modèle!A5,"")</f>
-        <v>Publication</v>
+        <v>Jeu de tests</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B5) &gt; 0, modèle!B5,""),IF(LEN(modèle!C5) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C5,IF(modèle!C5 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Le jeu de données de permet de tester l’ensemble des fonctionnalités.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D5) &gt; 0, modèle!D5,""),IF(LEN(modèle!E5) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E5,IF(modèle!E5 &gt; 1," points"," point")),""))</f>
@@ -853,7 +826,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F5) &gt; 0, modèle!F5,""),IF(LEN(modèle!G5) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G5,IF(modèle!G5 &gt; 1," points"," point")),""))</f>
-        <v>Le base de données est publiée. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>Le jeu de données de permet de tester partiellement les fonctionnalités.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H5) &gt; 0, modèle!H5,""),IF(LEN(modèle!I5) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I5,IF(modèle!I5 &gt; 1," points"," point")),""))</f>
@@ -861,17 +834,17 @@
       </c>
       <c r="F5" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J5) &gt; 0, modèle!J5,""),IF(LEN(modèle!K5) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K5,IF(modèle!K5 &gt; 1," points"," point")),""))</f>
-        <v>La base de données n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>Le jeu de données de permet de tester moins de 25% des fonctionnalités.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>IF(LEN(modèle!A6) &gt; 0, modèle!A6,"")</f>
-        <v>Jeu de tests</v>
+        <v>__Interface applicative (API) (40%)__ {: colspan=5}</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B6) &gt; 0, modèle!B6,""),IF(LEN(modèle!C6) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C6,IF(modèle!C6 &gt; 1," points"," point")),""))</f>
-        <v>Le jeu de données de permet de tester l’ensemble des fonctionnalités.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D6) &gt; 0, modèle!D6,""),IF(LEN(modèle!E6) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E6,IF(modèle!E6 &gt; 1," points"," point")),""))</f>
@@ -879,7 +852,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F6) &gt; 0, modèle!F6,""),IF(LEN(modèle!G6) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G6,IF(modèle!G6 &gt; 1," points"," point")),""))</f>
-        <v>Le jeu de données de permet de tester partiellement les fonctionnalités.&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v/>
       </c>
       <c r="E6" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H6) &gt; 0, modèle!H6,""),IF(LEN(modèle!I6) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I6,IF(modèle!I6 &gt; 1," points"," point")),""))</f>
@@ -887,77 +860,77 @@
       </c>
       <c r="F6" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J6) &gt; 0, modèle!J6,""),IF(LEN(modèle!K6) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K6,IF(modèle!K6 &gt; 1," points"," point")),""))</f>
-        <v>Le jeu de données de permet de tester moins de 25% des fonctionnalités.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(LEN(modèle!A7) &gt; 0, modèle!A7,"")</f>
-        <v>__Interface applicative (API) (40%)__ {: colspan=5}</v>
+        <v>Méthodes HTTP</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B7) &gt; 0, modèle!B7,""),IF(LEN(modèle!C7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C7,IF(modèle!C7 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;8 points</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D7) &gt; 0, modèle!D7,""),IF(LEN(modèle!E7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E7,IF(modèle!E7 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;6 points</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F7) &gt; 0, modèle!F7,""),IF(LEN(modèle!G7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G7,IF(modèle!G7 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H7) &gt; 0, modèle!H7,""),IF(LEN(modèle!I7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I7,IF(modèle!I7 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J7) &gt; 0, modèle!J7,""),IF(LEN(modèle!K7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K7,IF(modèle!K7 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="289" x14ac:dyDescent="0.2">
+        <v>L’interface applicative implémente __moins de 25%__ des méthodes HTTP demandées. &lt;br/&gt; (GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>IF(LEN(modèle!A8) &gt; 0, modèle!A8,"")</f>
-        <v>Méthodes HTTP</v>
+        <v>GET avec filtre</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B8) &gt; 0, modèle!B8,""),IF(LEN(modèle!C8) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C8,IF(modèle!C8 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;8 points</v>
+        <v>L’interface applicative implémente correctement un minimum de 2 méthodes GET avec filtres. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D8) &gt; 0, modèle!D8,""),IF(LEN(modèle!E8) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E8,IF(modèle!E8 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;6 points</v>
+        <v>L’interface applicative implémente partiellement un minimum de 2 méthodes GET avec filtres. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F8) &gt; 0, modèle!F8,""),IF(LEN(modèle!G8) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G8,IF(modèle!G8 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative implémente partiellement moins de 2 méthodes GET avec filtres. Ces requêtes sont peu pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H8) &gt; 0, modèle!H8,""),IF(LEN(modèle!I8) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I8,IF(modèle!I8 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="F8" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J8) &gt; 0, modèle!J8,""),IF(LEN(modèle!K8) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K8,IF(modèle!K8 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __moins de 25%__ des méthodes HTTP demandées. &lt;br/&gt; (GET, POST, PUT, PATCH, DELETE)&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>L’interface applicative n’implémente pas correctement de méthodes GET avec filtres, ou ces requêtes ne sont pas pertinentes au projet&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>IF(LEN(modèle!A9) &gt; 0, modèle!A9,"")</f>
-        <v>GET avec filtre</v>
+        <v>Validations natives</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B9) &gt; 0, modèle!B9,""),IF(LEN(modèle!C9) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C9,IF(modèle!C9 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente correctement un minimum de 2 méthodes GET avec filtres. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D9) &gt; 0, modèle!D9,""),IF(LEN(modèle!E9) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E9,IF(modèle!E9 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente partiellement un minimum de 2 méthodes GET avec filtres. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="D9" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F9) &gt; 0, modèle!F9,""),IF(LEN(modèle!G9) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G9,IF(modèle!G9 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente partiellement moins de 2 méthodes GET avec filtres. Ces requêtes sont peu pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’interface applicative contient des __validations natives__ partiellement appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H9) &gt; 0, modèle!H9,""),IF(LEN(modèle!I9) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I9,IF(modèle!I9 &gt; 1," points"," point")),""))</f>
@@ -965,25 +938,25 @@
       </c>
       <c r="F9" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J9) &gt; 0, modèle!J9,""),IF(LEN(modèle!K9) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K9,IF(modèle!K9 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’implémente pas correctement de méthodes GET avec filtres, ou ces requêtes ne sont pas pertinentes au projet&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+        <v>L’interface applicative ne contient pas de __validations natives__ appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>IF(LEN(modèle!A10) &gt; 0, modèle!A10,"")</f>
-        <v>GET avec transformation</v>
+        <v>Validations personnalisées</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B10) &gt; 0, modèle!B10,""),IF(LEN(modèle!C10) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C10,IF(modèle!C10 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente correctement un minimum de 2 méthodes GET avec transformations. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative contient au minimum 2 __validations personnalisées__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D10) &gt; 0, modèle!D10,""),IF(LEN(modèle!E10) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E10,IF(modèle!E10 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente partiellement un minimum de 2 méthodes GET avec transformations. Ces requêtes sont pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="D10" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F10) &gt; 0, modèle!F10,""),IF(LEN(modèle!G10) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G10,IF(modèle!G10 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente partiellement moins de 2 méthodes GET avec transformations. Ces requêtes sont peu pertinentes au projet.  &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’interface applicative contient au moins 1 __validation personnalisée__ appropriée aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H10) &gt; 0, modèle!H10,""),IF(LEN(modèle!I10) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I10,IF(modèle!I10 &gt; 1," points"," point")),""))</f>
@@ -991,17 +964,17 @@
       </c>
       <c r="F10" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J10) &gt; 0, modèle!J10,""),IF(LEN(modèle!K10) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K10,IF(modèle!K10 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’implémente pas correctement de méthodes GET avec transformations, ou ces requêtes ne sont pas pertinentes au projet&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’interface applicative ne contient pas de __validation personnalisée__ appropriée aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>IF(LEN(modèle!A11) &gt; 0, modèle!A11,"")</f>
-        <v>Validations natives</v>
+        <v>Application sécurisée</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B11) &gt; 0, modèle!B11,""),IF(LEN(modèle!C11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C11,IF(modèle!C11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des __validations natives__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;6 points</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D11) &gt; 0, modèle!D11,""),IF(LEN(modèle!E11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E11,IF(modèle!E11 &gt; 1," points"," point")),""))</f>
@@ -1009,7 +982,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F11) &gt; 0, modèle!F11,""),IF(LEN(modèle!G11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G11,IF(modèle!G11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des __validations natives__ partiellement appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H11) &gt; 0, modèle!H11,""),IF(LEN(modèle!I11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I11,IF(modèle!I11 &gt; 1," points"," point")),""))</f>
@@ -1017,17 +990,17 @@
       </c>
       <c r="F11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J11) &gt; 0, modèle!J11,""),IF(LEN(modèle!K11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K11,IF(modèle!K11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de __validations natives__ appropriées aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’interface applicative n’est pas __sécurisée__.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>IF(LEN(modèle!A12) &gt; 0, modèle!A12,"")</f>
-        <v>Validations personnalisées</v>
+        <v>Messages d'erreur</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B12) &gt; 0, modèle!B12,""),IF(LEN(modèle!C12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C12,IF(modèle!C12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient au minimum 2 __validations personnalisées__ appropriées aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D12) &gt; 0, modèle!D12,""),IF(LEN(modèle!E12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E12,IF(modèle!E12 &gt; 1," points"," point")),""))</f>
@@ -1035,7 +1008,7 @@
       </c>
       <c r="D12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F12) &gt; 0, modèle!F12,""),IF(LEN(modèle!G12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G12,IF(modèle!G12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient au moins 1 __validation personnalisée__ appropriée aux données représentées dans le schéma.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H12) &gt; 0, modèle!H12,""),IF(LEN(modèle!I12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I12,IF(modèle!I12 &gt; 1," points"," point")),""))</f>
@@ -1043,17 +1016,17 @@
       </c>
       <c r="F12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J12) &gt; 0, modèle!J12,""),IF(LEN(modèle!K12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K12,IF(modèle!K12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de __validation personnalisée__ appropriée aux données représentées dans le schéma&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’interface applicative ne contient pas de messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>IF(LEN(modèle!A13) &gt; 0, modèle!A13,"")</f>
-        <v>Application sécurisée</v>
+        <v>Publication</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B13) &gt; 0, modèle!B13,""),IF(LEN(modèle!C13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C13,IF(modèle!C13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;6 points</v>
+        <v>L’interface applicative est publiée et fonctionnelle. &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D13) &gt; 0, modèle!D13,""),IF(LEN(modèle!E13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E13,IF(modèle!E13 &gt; 1," points"," point")),""))</f>
@@ -1061,7 +1034,7 @@
       </c>
       <c r="D13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F13) &gt; 0, modèle!F13,""),IF(LEN(modèle!G13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G13,IF(modèle!G13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative n’est pas correctement publiée. &lt;br/&gt;Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H13) &gt; 0, modèle!H13,""),IF(LEN(modèle!I13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I13,IF(modèle!I13 &gt; 1," points"," point")),""))</f>
@@ -1069,17 +1042,17 @@
       </c>
       <c r="F13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J13) &gt; 0, modèle!J13,""),IF(LEN(modèle!K13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K13,IF(modèle!K13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas __sécurisée__.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’interface applicative n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>IF(LEN(modèle!A14) &gt; 0, modèle!A14,"")</f>
-        <v>Messages d'erreur</v>
+        <v>Documentation</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B14) &gt; 0, modèle!B14,""),IF(LEN(modèle!C14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C14,IF(modèle!C14 &gt; 1," points"," point")),""))</f>
-        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D14) &gt; 0, modèle!D14,""),IF(LEN(modèle!E14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E14,IF(modèle!E14 &gt; 1," points"," point")),""))</f>
@@ -1087,7 +1060,7 @@
       </c>
       <c r="D14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F14) &gt; 0, modèle!F14,""),IF(LEN(modèle!G14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G14,IF(modèle!G14 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H14) &gt; 0, modèle!H14,""),IF(LEN(modèle!I14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I14,IF(modèle!I14 &gt; 1," points"," point")),""))</f>
@@ -1095,17 +1068,17 @@
       </c>
       <c r="F14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J14) &gt; 0, modèle!J14,""),IF(LEN(modèle!K14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K14,IF(modèle!K14 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative ne contient pas de messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>IF(LEN(modèle!A15) &gt; 0, modèle!A15,"")</f>
-        <v>Publication</v>
+        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B15) &gt; 0, modèle!B15,""),IF(LEN(modèle!C15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C15,IF(modèle!C15 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est publiée et fonctionnelle. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D15) &gt; 0, modèle!D15,""),IF(LEN(modèle!E15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E15,IF(modèle!E15 &gt; 1," points"," point")),""))</f>
@@ -1113,7 +1086,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F15) &gt; 0, modèle!F15,""),IF(LEN(modèle!G15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G15,IF(modèle!G15 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée. &lt;br/&gt;Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v/>
       </c>
       <c r="E15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H15) &gt; 0, modèle!H15,""),IF(LEN(modèle!I15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I15,IF(modèle!I15 &gt; 1," points"," point")),""))</f>
@@ -1121,17 +1094,17 @@
       </c>
       <c r="F15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J15) &gt; 0, modèle!J15,""),IF(LEN(modèle!K15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K15,IF(modèle!K15 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f>IF(LEN(modèle!A16) &gt; 0, modèle!A16,"")</f>
-        <v>Documentation</v>
+        <v>__Application Web (50%)__ {: colspan=5}</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B16) &gt; 0, modèle!B16,""),IF(LEN(modèle!C16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C16,IF(modèle!C16 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D16) &gt; 0, modèle!D16,""),IF(LEN(modèle!E16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E16,IF(modèle!E16 &gt; 1," points"," point")),""))</f>
@@ -1139,7 +1112,7 @@
       </c>
       <c r="D16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F16) &gt; 0, modèle!F16,""),IF(LEN(modèle!G16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G16,IF(modèle!G16 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="E16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H16) &gt; 0, modèle!H16,""),IF(LEN(modèle!I16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I16,IF(modèle!I16 &gt; 1," points"," point")),""))</f>
@@ -1147,17 +1120,17 @@
       </c>
       <c r="F16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J16) &gt; 0, modèle!J16,""),IF(LEN(modèle!K16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K16,IF(modèle!K16 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>IF(LEN(modèle!A17) &gt; 0, modèle!A17,"")</f>
-        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
+        <v>Composants</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B17) &gt; 0, modèle!B17,""),IF(LEN(modèle!C17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C17,IF(modèle!C17 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D17) &gt; 0, modèle!D17,""),IF(LEN(modèle!E17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E17,IF(modèle!E17 &gt; 1," points"," point")),""))</f>
@@ -1165,33 +1138,33 @@
       </c>
       <c r="D17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F17) &gt; 0, modèle!F17,""),IF(LEN(modèle!G17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G17,IF(modèle!G17 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H17) &gt; 0, modèle!H17,""),IF(LEN(modèle!I17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I17,IF(modèle!I17 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J17) &gt; 0, modèle!J17,""),IF(LEN(modèle!K17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K17,IF(modèle!K17 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(LEN(modèle!A18) &gt; 0, modèle!A18,"")</f>
-        <v>__Application Web (50%)__ {: colspan=5}</v>
+        <v>Hooks</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B18) &gt; 0, modèle!B18,""),IF(LEN(modèle!C18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C18,IF(modèle!C18 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D18) &gt; 0, modèle!D18,""),IF(LEN(modèle!E18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E18,IF(modèle!E18 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F18) &gt; 0, modèle!F18,""),IF(LEN(modèle!G18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G18,IF(modèle!G18 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H18) &gt; 0, modèle!H18,""),IF(LEN(modèle!I18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I18,IF(modèle!I18 &gt; 1," points"," point")),""))</f>
@@ -1199,51 +1172,51 @@
       </c>
       <c r="F18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J18) &gt; 0, modèle!J18,""),IF(LEN(modèle!K18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K18,IF(modèle!K18 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(LEN(modèle!A19) &gt; 0, modèle!A19,"")</f>
-        <v>Composants</v>
+        <v>Méthodes HTTP</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B19) &gt; 0, modèle!B19,""),IF(LEN(modèle!C19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C19,IF(modèle!C19 &gt; 1," points"," point")),""))</f>
-        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D19) &gt; 0, modèle!D19,""),IF(LEN(modèle!E19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E19,IF(modèle!E19 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F19) &gt; 0, modèle!F19,""),IF(LEN(modèle!G19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G19,IF(modèle!G19 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H19) &gt; 0, modèle!H19,""),IF(LEN(modèle!I19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I19,IF(modèle!I19 &gt; 1," points"," point")),""))</f>
-        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="F19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J19) &gt; 0, modèle!J19,""),IF(LEN(modèle!K19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K19,IF(modèle!K19 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(LEN(modèle!A20) &gt; 0, modèle!A20,"")</f>
-        <v>Hooks</v>
+        <v>Validations</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B20) &gt; 0, modèle!B20,""),IF(LEN(modèle!C20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C20,IF(modèle!C20 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application contient des validations appropriées avec messages à l'utilisateur dans l'interface graphique.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D20) &gt; 0, modèle!D20,""),IF(LEN(modèle!E20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E20,IF(modèle!E20 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="D20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F20) &gt; 0, modèle!F20,""),IF(LEN(modèle!G20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G20,IF(modèle!G20 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application contient des validations partiellement appropriées qui ont des messages affichés à l'utilisateur.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H20) &gt; 0, modèle!H20,""),IF(LEN(modèle!I20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I20,IF(modèle!I20 &gt; 1," points"," point")),""))</f>
@@ -1251,43 +1224,43 @@
       </c>
       <c r="F20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J20) &gt; 0, modèle!J20,""),IF(LEN(modèle!K20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K20,IF(modèle!K20 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+        <v>L’application ne contient pas de validations appropriées ou ne sont pas affichées à l'utilisateur.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(LEN(modèle!A21) &gt; 0, modèle!A21,"")</f>
-        <v>Méthodes HTTP</v>
+        <v>Visuel</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B21) &gt; 0, modèle!B21,""),IF(LEN(modèle!C21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C21,IF(modèle!C21 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
+        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D21) &gt; 0, modèle!D21,""),IF(LEN(modèle!E21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E21,IF(modèle!E21 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
+        <v/>
       </c>
       <c r="D21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F21) &gt; 0, modèle!F21,""),IF(LEN(modèle!G21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G21,IF(modèle!G21 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
+        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H21) &gt; 0, modèle!H21,""),IF(LEN(modèle!I21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I21,IF(modèle!I21 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="F21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J21) &gt; 0, modèle!J21,""),IF(LEN(modèle!K21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K21,IF(modèle!K21 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f>IF(LEN(modèle!A22) &gt; 0, modèle!A22,"")</f>
-        <v>Validations</v>
+        <v>Application sécurisée</v>
       </c>
       <c r="B22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B22) &gt; 0, modèle!B22,""),IF(LEN(modèle!C22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C22,IF(modèle!C22 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations appropriées.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D22) &gt; 0, modèle!D22,""),IF(LEN(modèle!E22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E22,IF(modèle!E22 &gt; 1," points"," point")),""))</f>
@@ -1295,7 +1268,7 @@
       </c>
       <c r="D22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F22) &gt; 0, modèle!F22,""),IF(LEN(modèle!G22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G22,IF(modèle!G22 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations partiellement appropriées.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H22) &gt; 0, modèle!H22,""),IF(LEN(modèle!I22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I22,IF(modèle!I22 &gt; 1," points"," point")),""))</f>
@@ -1303,17 +1276,17 @@
       </c>
       <c r="F22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J22) &gt; 0, modèle!J22,""),IF(LEN(modèle!K22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K22,IF(modèle!K22 &gt; 1," points"," point")),""))</f>
-        <v>L’application ne contient pas de validations appropriées.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>IF(LEN(modèle!A23) &gt; 0, modèle!A23,"")</f>
-        <v>Visuel</v>
+        <v>Internationalisation</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B23) &gt; 0, modèle!B23,""),IF(LEN(modèle!C23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C23,IF(modèle!C23 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application est entièrement internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D23) &gt; 0, modèle!D23,""),IF(LEN(modèle!E23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E23,IF(modèle!E23 &gt; 1," points"," point")),""))</f>
@@ -1321,7 +1294,7 @@
       </c>
       <c r="D23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F23) &gt; 0, modèle!F23,""),IF(LEN(modèle!G23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G23,IF(modèle!G23 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est partiellement internationaliséeen Français et en Anglais&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H23) &gt; 0, modèle!H23,""),IF(LEN(modèle!I23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I23,IF(modèle!I23 &gt; 1," points"," point")),""))</f>
@@ -1329,17 +1302,17 @@
       </c>
       <c r="F23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J23) &gt; 0, modèle!J23,""),IF(LEN(modèle!K23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K23,IF(modèle!K23 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f>IF(LEN(modèle!A24) &gt; 0, modèle!A24,"")</f>
-        <v>Application sécurisée</v>
+        <v>Organisation visuelle</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B24) &gt; 0, modèle!B24,""),IF(LEN(modèle!C24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C24,IF(modèle!C24 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D24) &gt; 0, modèle!D24,""),IF(LEN(modèle!E24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E24,IF(modèle!E24 &gt; 1," points"," point")),""))</f>
@@ -1347,7 +1320,7 @@
       </c>
       <c r="D24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F24) &gt; 0, modèle!F24,""),IF(LEN(modèle!G24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G24,IF(modèle!G24 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H24) &gt; 0, modèle!H24,""),IF(LEN(modèle!I24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I24,IF(modèle!I24 &gt; 1," points"," point")),""))</f>
@@ -1355,17 +1328,17 @@
       </c>
       <c r="F24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J24) &gt; 0, modèle!J24,""),IF(LEN(modèle!K24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K24,IF(modèle!K24 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f>IF(LEN(modèle!A25) &gt; 0, modèle!A25,"")</f>
-        <v>Internationalisation</v>
+        <v>Navigation</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B25) &gt; 0, modèle!B25,""),IF(LEN(modèle!C25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C25,IF(modèle!C25 &gt; 1," points"," point")),""))</f>
-        <v>L’application est entièrement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D25) &gt; 0, modèle!D25,""),IF(LEN(modèle!E25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E25,IF(modèle!E25 &gt; 1," points"," point")),""))</f>
@@ -1373,7 +1346,7 @@
       </c>
       <c r="D25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F25) &gt; 0, modèle!F25,""),IF(LEN(modèle!G25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G25,IF(modèle!G25 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H25) &gt; 0, modèle!H25,""),IF(LEN(modèle!I25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I25,IF(modèle!I25 &gt; 1," points"," point")),""))</f>
@@ -1381,17 +1354,17 @@
       </c>
       <c r="F25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J25) &gt; 0, modèle!J25,""),IF(LEN(modèle!K25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K25,IF(modèle!K25 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas internationalisée dans un minimum de 2 langues&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
         <f>IF(LEN(modèle!A26) &gt; 0, modèle!A26,"")</f>
-        <v>Organisation visuelle</v>
+        <v>PWA</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B26) &gt; 0, modèle!B26,""),IF(LEN(modèle!C26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C26,IF(modèle!C26 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 75% des exigences.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D26) &gt; 0, modèle!D26,""),IF(LEN(modèle!E26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E26,IF(modèle!E26 &gt; 1," points"," point")),""))</f>
@@ -1399,7 +1372,7 @@
       </c>
       <c r="D26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F26) &gt; 0, modèle!F26,""),IF(LEN(modèle!G26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G26,IF(modèle!G26 &gt; 1," points"," point")),""))</f>
-        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 50% des exigences.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H26) &gt; 0, modèle!H26,""),IF(LEN(modèle!I26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I26,IF(modèle!I26 &gt; 1," points"," point")),""))</f>
@@ -1407,17 +1380,17 @@
       </c>
       <c r="F26" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J26) &gt; 0, modèle!J26,""),IF(LEN(modèle!K26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K26,IF(modèle!K26 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’application est configurée en tant qu’application progressive (PWA) ou répond à moins de 50% des exigences.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
         <f>IF(LEN(modèle!A27) &gt; 0, modèle!A27,"")</f>
-        <v>Navigation</v>
+        <v>Publication</v>
       </c>
       <c r="B27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B27) &gt; 0, modèle!B27,""),IF(LEN(modèle!C27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C27,IF(modèle!C27 &gt; 1," points"," point")),""))</f>
-        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D27) &gt; 0, modèle!D27,""),IF(LEN(modèle!E27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E27,IF(modèle!E27 &gt; 1," points"," point")),""))</f>
@@ -1425,7 +1398,7 @@
       </c>
       <c r="D27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F27) &gt; 0, modèle!F27,""),IF(LEN(modèle!G27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G27,IF(modèle!G27 &gt; 1," points"," point")),""))</f>
-        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H27) &gt; 0, modèle!H27,""),IF(LEN(modèle!I27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I27,IF(modèle!I27 &gt; 1," points"," point")),""))</f>
@@ -1433,17 +1406,17 @@
       </c>
       <c r="F27" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J27) &gt; 0, modèle!J27,""),IF(LEN(modèle!K27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K27,IF(modèle!K27 &gt; 1," points"," point")),""))</f>
-        <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
         <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
-        <v>PWA</v>
+        <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 75% des exigences.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="C28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
@@ -1451,7 +1424,7 @@
       </c>
       <c r="D28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 50% des exigences.&lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v/>
       </c>
       <c r="E28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
@@ -1459,58 +1432,6 @@
       </c>
       <c r="F28" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
-        <v>L’application est configurée en tant qu’application progressive (PWA) ou répond à moins de 50% des exigences.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="str">
-        <f>IF(LEN(modèle!A29) &gt; 0, modèle!A29,"")</f>
-        <v>Publication</v>
-      </c>
-      <c r="B29" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B29) &gt; 0, modèle!B29,""),IF(LEN(modèle!C29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C29,IF(modèle!C29 &gt; 1," points"," point")),""))</f>
-        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
-      </c>
-      <c r="C29" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D29) &gt; 0, modèle!D29,""),IF(LEN(modèle!E29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E29,IF(modèle!E29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="D29" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F29) &gt; 0, modèle!F29,""),IF(LEN(modèle!G29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G29,IF(modèle!G29 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
-      </c>
-      <c r="E29" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H29) &gt; 0, modèle!H29,""),IF(LEN(modèle!I29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I29,IF(modèle!I29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="F29" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J29) &gt; 0, modèle!J29,""),IF(LEN(modèle!K29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K29,IF(modèle!K29 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="str">
-        <f>IF(LEN(modèle!A30) &gt; 0, modèle!A30,"")</f>
-        <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
-      </c>
-      <c r="B30" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B30) &gt; 0, modèle!B30,""),IF(LEN(modèle!C30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C30,IF(modèle!C30 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="C30" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D30) &gt; 0, modèle!D30,""),IF(LEN(modèle!E30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E30,IF(modèle!E30 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="D30" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F30) &gt; 0, modèle!F30,""),IF(LEN(modèle!G30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G30,IF(modèle!G30 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="E30" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H30) &gt; 0, modèle!H30,""),IF(LEN(modèle!I30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I30,IF(modèle!I30 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="F30" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J30) &gt; 0, modèle!J30,""),IF(LEN(modèle!K30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K30,IF(modèle!K30 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
@@ -1521,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004F3CC3-38A6-1349-9E0D-D575CD7A9164}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1564,78 +1485,78 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="M3">
-        <f>MAX(C3,E3,G3,I3)</f>
-        <v>2</v>
+        <f t="shared" ref="M3:M18" si="0">MAX(C3,E3,G3,I3)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M20" si="0">MAX(C4,E4,G4,I4)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -1650,190 +1571,184 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>62</v>
+      <c r="J7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1845,49 +1760,49 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>52</v>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1897,228 +1812,228 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
+    <row r="15" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="J16" t="s">
-        <v>59</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" ref="M19:M27" si="1">MAX(C19,E19,G19,I19)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20">
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="F20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
       <c r="J20" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G21">
-        <v>7</v>
-      </c>
-      <c r="H21" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21">
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M21:M29" si="1">MAX(C21,E21,G21,I21)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" t="s">
-        <v>75</v>
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G22">
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -2128,105 +2043,105 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
       </c>
       <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="F24" t="s">
-        <v>84</v>
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>79</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2236,63 +2151,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="F28" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="J28" t="s">
-        <v>100</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="J29" t="s">
-        <v>103</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>104</v>
+    <row r="28" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout tests unitaires au projet intégrateur
</commit_message>
<xml_diff>
--- a/template/grille_correction.xlsx
+++ b/template/grille_correction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7D37F-B90C-D441-802F-464E4783595F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10054A6-6797-6C4C-983E-CE790D424324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>Élément</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>L’application est entièrement internationalisée en Français et en Anglais</t>
+  </si>
+  <si>
+    <t>Tests unitaires automatisés</t>
+  </si>
+  <si>
+    <t>L'ensemble des méthodes HTTP implémentés et des validations sont testées</t>
+  </si>
+  <si>
+    <t>Les tests unitaires ne couvrent que __75%__ des méthodes HTTP et validations</t>
+  </si>
+  <si>
+    <t>Les tests unitaires ne couvrent que __50%__ des méthodes HTTP et validations</t>
+  </si>
+  <si>
+    <t>Les tests unitaires couvrent moins de  __25%__ des méthodes HTTP et validations</t>
+  </si>
+  <si>
+    <t>Les tests unitaires ne couvrent que __25%__ des méthodes HTTP et validations</t>
   </si>
 </sst>
 </file>
@@ -699,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,7 +792,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F3) &gt; 0, modèle!F3,""),IF(LEN(modèle!G3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G3,IF(modèle!G3 &gt; 1," points"," point")),""))</f>
-        <v>3 à 5 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>3 à 5 éléments du schéma ne répondent pas aux exigences demandées&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H3) &gt; 0, modèle!H3,""),IF(LEN(modèle!I3) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I3,IF(modèle!I3 &gt; 1," points"," point")),""))</f>
@@ -863,26 +881,26 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="289" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(LEN(modèle!A7) &gt; 0, modèle!A7,"")</f>
         <v>Méthodes HTTP</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B7) &gt; 0, modèle!B7,""),IF(LEN(modèle!C7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C7,IF(modèle!C7 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;8 points</v>
+        <v>L’interface applicative implémente __correctement l’ensemble__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D7) &gt; 0, modèle!D7,""),IF(LEN(modèle!E7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E7,IF(modèle!E7 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;6 points</v>
+        <v>L’interface applicative implémente __correctement 75%__ des méthodes HTTP demandées.  &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F7) &gt; 0, modèle!F7,""),IF(LEN(modèle!G7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G7,IF(modèle!G7 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative implémente __correctement 50%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H7) &gt; 0, modèle!H7,""),IF(LEN(modèle!I7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I7,IF(modèle!I7 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’interface applicative implémente __correctement 25%__ des méthodes HTTP demandées. &lt;br/&gt;(GET, POST, PUT, DELETE)&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J7) &gt; 0, modèle!J7,""),IF(LEN(modèle!K7) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K7,IF(modèle!K7 &gt; 1," points"," point")),""))</f>
@@ -974,7 +992,7 @@
       </c>
       <c r="B11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B11) &gt; 0, modèle!B11,""),IF(LEN(modèle!C11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C11,IF(modèle!C11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;6 points</v>
+        <v>L’interface applicative est correctement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D11) &gt; 0, modèle!D11,""),IF(LEN(modèle!E11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E11,IF(modèle!E11 &gt; 1," points"," point")),""))</f>
@@ -982,7 +1000,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F11) &gt; 0, modèle!F11,""),IF(LEN(modèle!G11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G11,IF(modèle!G11 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L’interface applicative est partiellement __sécurisée__.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H11) &gt; 0, modèle!H11,""),IF(LEN(modèle!I11) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I11,IF(modèle!I11 &gt; 1," points"," point")),""))</f>
@@ -1000,7 +1018,7 @@
       </c>
       <c r="B12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B12) &gt; 0, modèle!B12,""),IF(LEN(modèle!C12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C12,IF(modèle!C12 &gt; 1," points"," point")),""))</f>
-        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>Les messages d’erreur sont personnalisés en français.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D12) &gt; 0, modèle!D12,""),IF(LEN(modèle!E12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E12,IF(modèle!E12 &gt; 1," points"," point")),""))</f>
@@ -1008,7 +1026,7 @@
       </c>
       <c r="D12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F12) &gt; 0, modèle!F12,""),IF(LEN(modèle!G12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G12,IF(modèle!G12 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’interface applicative contient des messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H12) &gt; 0, modèle!H12,""),IF(LEN(modèle!I12) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I12,IF(modèle!I12 &gt; 1," points"," point")),""))</f>
@@ -1019,419 +1037,419 @@
         <v>L’interface applicative ne contient pas de messages d’erreurs appropriés.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>IF(LEN(modèle!A13) &gt; 0, modèle!A13,"")</f>
-        <v>Publication</v>
+        <v>Tests unitaires automatisés</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B13) &gt; 0, modèle!B13,""),IF(LEN(modèle!C13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C13,IF(modèle!C13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative est publiée et fonctionnelle. &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L'ensemble des méthodes HTTP implémentés et des validations sont testées&lt;br/&gt;&lt;br/&gt;6 points</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D13) &gt; 0, modèle!D13,""),IF(LEN(modèle!E13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E13,IF(modèle!E13 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les tests unitaires ne couvrent que __75%__ des méthodes HTTP et validations&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F13) &gt; 0, modèle!F13,""),IF(LEN(modèle!G13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G13,IF(modèle!G13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée. &lt;br/&gt;Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
+        <v>Les tests unitaires ne couvrent que __50%__ des méthodes HTTP et validations&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H13) &gt; 0, modèle!H13,""),IF(LEN(modèle!I13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I13,IF(modèle!I13 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>Les tests unitaires ne couvrent que __25%__ des méthodes HTTP et validations&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J13) &gt; 0, modèle!J13,""),IF(LEN(modèle!K13) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K13,IF(modèle!K13 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>Les tests unitaires couvrent moins de  __25%__ des méthodes HTTP et validations&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
-        <f>IF(LEN(modèle!A14) &gt; 0, modèle!A14,"")</f>
+        <f>IF(LEN(modèle!A15) &gt; 0, modèle!A15,"")</f>
         <v>Documentation</v>
       </c>
       <c r="B14" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B14) &gt; 0, modèle!B14,""),IF(LEN(modèle!C14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C14,IF(modèle!C14 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B15) &gt; 0, modèle!B15,""),IF(LEN(modèle!C15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C15,IF(modèle!C15 &gt; 1," points"," point")),""))</f>
         <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D14) &gt; 0, modèle!D14,""),IF(LEN(modèle!E14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E14,IF(modèle!E14 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D15) &gt; 0, modèle!D15,""),IF(LEN(modèle!E15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E15,IF(modèle!E15 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D14" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F14) &gt; 0, modèle!F14,""),IF(LEN(modèle!G14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G14,IF(modèle!G14 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F15) &gt; 0, modèle!F15,""),IF(LEN(modèle!G15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G15,IF(modèle!G15 &gt; 1," points"," point")),""))</f>
         <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H14) &gt; 0, modèle!H14,""),IF(LEN(modèle!I14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I14,IF(modèle!I14 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H15) &gt; 0, modèle!H15,""),IF(LEN(modèle!I15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I15,IF(modèle!I15 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F14" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J14) &gt; 0, modèle!J14,""),IF(LEN(modèle!K14) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K14,IF(modèle!K14 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J15) &gt; 0, modèle!J15,""),IF(LEN(modèle!K15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K15,IF(modèle!K15 &gt; 1," points"," point")),""))</f>
         <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
-        <f>IF(LEN(modèle!A15) &gt; 0, modèle!A15,"")</f>
+        <f>IF(LEN(modèle!A16) &gt; 0, modèle!A16,"")</f>
         <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B15) &gt; 0, modèle!B15,""),IF(LEN(modèle!C15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C15,IF(modèle!C15 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B16) &gt; 0, modèle!B16,""),IF(LEN(modèle!C16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C16,IF(modèle!C16 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D15) &gt; 0, modèle!D15,""),IF(LEN(modèle!E15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E15,IF(modèle!E15 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D16) &gt; 0, modèle!D16,""),IF(LEN(modèle!E16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E16,IF(modèle!E16 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D15" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F15) &gt; 0, modèle!F15,""),IF(LEN(modèle!G15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G15,IF(modèle!G15 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F16) &gt; 0, modèle!F16,""),IF(LEN(modèle!G16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G16,IF(modèle!G16 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="E15" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H15) &gt; 0, modèle!H15,""),IF(LEN(modèle!I15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I15,IF(modèle!I15 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H16) &gt; 0, modèle!H16,""),IF(LEN(modèle!I16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I16,IF(modèle!I16 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F15" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J15) &gt; 0, modèle!J15,""),IF(LEN(modèle!K15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K15,IF(modèle!K15 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J16) &gt; 0, modèle!J16,""),IF(LEN(modèle!K16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K16,IF(modèle!K16 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
-        <f>IF(LEN(modèle!A16) &gt; 0, modèle!A16,"")</f>
+        <f>IF(LEN(modèle!A17) &gt; 0, modèle!A17,"")</f>
         <v>__Application Web (50%)__ {: colspan=5}</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B16) &gt; 0, modèle!B16,""),IF(LEN(modèle!C16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C16,IF(modèle!C16 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B17) &gt; 0, modèle!B17,""),IF(LEN(modèle!C17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C17,IF(modèle!C17 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D16) &gt; 0, modèle!D16,""),IF(LEN(modèle!E16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E16,IF(modèle!E16 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D17) &gt; 0, modèle!D17,""),IF(LEN(modèle!E17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E17,IF(modèle!E17 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D16" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F16) &gt; 0, modèle!F16,""),IF(LEN(modèle!G16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G16,IF(modèle!G16 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F17) &gt; 0, modèle!F17,""),IF(LEN(modèle!G17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G17,IF(modèle!G17 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="E16" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H16) &gt; 0, modèle!H16,""),IF(LEN(modèle!I16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I16,IF(modèle!I16 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H17) &gt; 0, modèle!H17,""),IF(LEN(modèle!I17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I17,IF(modèle!I17 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F16" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J16) &gt; 0, modèle!J16,""),IF(LEN(modèle!K16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K16,IF(modèle!K16 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J17) &gt; 0, modèle!J17,""),IF(LEN(modèle!K17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K17,IF(modèle!K17 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
-        <f>IF(LEN(modèle!A17) &gt; 0, modèle!A17,"")</f>
+        <f>IF(LEN(modèle!A18) &gt; 0, modèle!A18,"")</f>
         <v>Composants</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B17) &gt; 0, modèle!B17,""),IF(LEN(modèle!C17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C17,IF(modèle!C17 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B18) &gt; 0, modèle!B18,""),IF(LEN(modèle!C18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C18,IF(modèle!C18 &gt; 1," points"," point")),""))</f>
         <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D17) &gt; 0, modèle!D17,""),IF(LEN(modèle!E17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E17,IF(modèle!E17 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D18) &gt; 0, modèle!D18,""),IF(LEN(modèle!E18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E18,IF(modèle!E18 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D17" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F17) &gt; 0, modèle!F17,""),IF(LEN(modèle!G17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G17,IF(modèle!G17 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F18) &gt; 0, modèle!F18,""),IF(LEN(modèle!G18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G18,IF(modèle!G18 &gt; 1," points"," point")),""))</f>
         <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H17) &gt; 0, modèle!H17,""),IF(LEN(modèle!I17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I17,IF(modèle!I17 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H18) &gt; 0, modèle!H18,""),IF(LEN(modèle!I18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I18,IF(modèle!I18 &gt; 1," points"," point")),""))</f>
         <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J17) &gt; 0, modèle!J17,""),IF(LEN(modèle!K17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K17,IF(modèle!K17 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J18) &gt; 0, modèle!J18,""),IF(LEN(modèle!K18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K18,IF(modèle!K18 &gt; 1," points"," point")),""))</f>
         <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
-        <f>IF(LEN(modèle!A18) &gt; 0, modèle!A18,"")</f>
+        <f>IF(LEN(modèle!A19) &gt; 0, modèle!A19,"")</f>
         <v>Hooks</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B18) &gt; 0, modèle!B18,""),IF(LEN(modèle!C18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C18,IF(modèle!C18 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B19) &gt; 0, modèle!B19,""),IF(LEN(modèle!C19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C19,IF(modèle!C19 &gt; 1," points"," point")),""))</f>
         <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D18) &gt; 0, modèle!D18,""),IF(LEN(modèle!E18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E18,IF(modèle!E18 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D19) &gt; 0, modèle!D19,""),IF(LEN(modèle!E19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E19,IF(modèle!E19 &gt; 1," points"," point")),""))</f>
         <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F18) &gt; 0, modèle!F18,""),IF(LEN(modèle!G18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G18,IF(modèle!G18 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F19) &gt; 0, modèle!F19,""),IF(LEN(modèle!G19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G19,IF(modèle!G19 &gt; 1," points"," point")),""))</f>
         <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H18) &gt; 0, modèle!H18,""),IF(LEN(modèle!I18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I18,IF(modèle!I18 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H19) &gt; 0, modèle!H19,""),IF(LEN(modèle!I19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I19,IF(modèle!I19 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F18" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J18) &gt; 0, modèle!J18,""),IF(LEN(modèle!K18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K18,IF(modèle!K18 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J19) &gt; 0, modèle!J19,""),IF(LEN(modèle!K19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K19,IF(modèle!K19 &gt; 1," points"," point")),""))</f>
         <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
-        <f>IF(LEN(modèle!A19) &gt; 0, modèle!A19,"")</f>
+        <f>IF(LEN(modèle!A20) &gt; 0, modèle!A20,"")</f>
         <v>Méthodes HTTP</v>
       </c>
       <c r="B19" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B19) &gt; 0, modèle!B19,""),IF(LEN(modèle!C19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C19,IF(modèle!C19 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B20) &gt; 0, modèle!B20,""),IF(LEN(modèle!C20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C20,IF(modèle!C20 &gt; 1," points"," point")),""))</f>
         <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D19) &gt; 0, modèle!D19,""),IF(LEN(modèle!E19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E19,IF(modèle!E19 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D20) &gt; 0, modèle!D20,""),IF(LEN(modèle!E20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E20,IF(modèle!E20 &gt; 1," points"," point")),""))</f>
         <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F19) &gt; 0, modèle!F19,""),IF(LEN(modèle!G19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G19,IF(modèle!G19 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F20) &gt; 0, modèle!F20,""),IF(LEN(modèle!G20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G20,IF(modèle!G20 &gt; 1," points"," point")),""))</f>
         <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
       </c>
       <c r="E19" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H19) &gt; 0, modèle!H19,""),IF(LEN(modèle!I19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I19,IF(modèle!I19 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H20) &gt; 0, modèle!H20,""),IF(LEN(modèle!I20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I20,IF(modèle!I20 &gt; 1," points"," point")),""))</f>
         <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J19) &gt; 0, modèle!J19,""),IF(LEN(modèle!K19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K19,IF(modèle!K19 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J20) &gt; 0, modèle!J20,""),IF(LEN(modèle!K20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K20,IF(modèle!K20 &gt; 1," points"," point")),""))</f>
         <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
-        <f>IF(LEN(modèle!A20) &gt; 0, modèle!A20,"")</f>
+        <f>IF(LEN(modèle!A21) &gt; 0, modèle!A21,"")</f>
         <v>Validations</v>
       </c>
       <c r="B20" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B20) &gt; 0, modèle!B20,""),IF(LEN(modèle!C20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C20,IF(modèle!C20 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B21) &gt; 0, modèle!B21,""),IF(LEN(modèle!C21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C21,IF(modèle!C21 &gt; 1," points"," point")),""))</f>
         <v>L’application contient des validations appropriées avec messages à l'utilisateur dans l'interface graphique.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D20) &gt; 0, modèle!D20,""),IF(LEN(modèle!E20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E20,IF(modèle!E20 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D21) &gt; 0, modèle!D21,""),IF(LEN(modèle!E21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E21,IF(modèle!E21 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D20" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F20) &gt; 0, modèle!F20,""),IF(LEN(modèle!G20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G20,IF(modèle!G20 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F21) &gt; 0, modèle!F21,""),IF(LEN(modèle!G21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G21,IF(modèle!G21 &gt; 1," points"," point")),""))</f>
         <v>L’application contient des validations partiellement appropriées qui ont des messages affichés à l'utilisateur.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H20) &gt; 0, modèle!H20,""),IF(LEN(modèle!I20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I20,IF(modèle!I20 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H21) &gt; 0, modèle!H21,""),IF(LEN(modèle!I21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I21,IF(modèle!I21 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F20" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J20) &gt; 0, modèle!J20,""),IF(LEN(modèle!K20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K20,IF(modèle!K20 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J21) &gt; 0, modèle!J21,""),IF(LEN(modèle!K21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K21,IF(modèle!K21 &gt; 1," points"," point")),""))</f>
         <v>L’application ne contient pas de validations appropriées ou ne sont pas affichées à l'utilisateur.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
-        <f>IF(LEN(modèle!A21) &gt; 0, modèle!A21,"")</f>
+        <f>IF(LEN(modèle!A22) &gt; 0, modèle!A22,"")</f>
         <v>Visuel</v>
       </c>
       <c r="B21" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B21) &gt; 0, modèle!B21,""),IF(LEN(modèle!C21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C21,IF(modèle!C21 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B22) &gt; 0, modèle!B22,""),IF(LEN(modèle!C22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C22,IF(modèle!C22 &gt; 1," points"," point")),""))</f>
         <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D21) &gt; 0, modèle!D21,""),IF(LEN(modèle!E21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E21,IF(modèle!E21 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D22) &gt; 0, modèle!D22,""),IF(LEN(modèle!E22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E22,IF(modèle!E22 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D21" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F21) &gt; 0, modèle!F21,""),IF(LEN(modèle!G21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G21,IF(modèle!G21 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F22) &gt; 0, modèle!F22,""),IF(LEN(modèle!G22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G22,IF(modèle!G22 &gt; 1," points"," point")),""))</f>
         <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E21" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H21) &gt; 0, modèle!H21,""),IF(LEN(modèle!I21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I21,IF(modèle!I21 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H22) &gt; 0, modèle!H22,""),IF(LEN(modèle!I22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I22,IF(modèle!I22 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F21" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J21) &gt; 0, modèle!J21,""),IF(LEN(modèle!K21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K21,IF(modèle!K21 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J22) &gt; 0, modèle!J22,""),IF(LEN(modèle!K22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K22,IF(modèle!K22 &gt; 1," points"," point")),""))</f>
         <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
-        <f>IF(LEN(modèle!A22) &gt; 0, modèle!A22,"")</f>
+        <f>IF(LEN(modèle!A23) &gt; 0, modèle!A23,"")</f>
         <v>Application sécurisée</v>
       </c>
       <c r="B22" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B22) &gt; 0, modèle!B22,""),IF(LEN(modèle!C22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C22,IF(modèle!C22 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B23) &gt; 0, modèle!B23,""),IF(LEN(modèle!C23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C23,IF(modèle!C23 &gt; 1," points"," point")),""))</f>
         <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D22) &gt; 0, modèle!D22,""),IF(LEN(modèle!E22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E22,IF(modèle!E22 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D23) &gt; 0, modèle!D23,""),IF(LEN(modèle!E23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E23,IF(modèle!E23 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D22" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F22) &gt; 0, modèle!F22,""),IF(LEN(modèle!G22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G22,IF(modèle!G22 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F23) &gt; 0, modèle!F23,""),IF(LEN(modèle!G23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G23,IF(modèle!G23 &gt; 1," points"," point")),""))</f>
         <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E22" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H22) &gt; 0, modèle!H22,""),IF(LEN(modèle!I22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I22,IF(modèle!I22 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H23) &gt; 0, modèle!H23,""),IF(LEN(modèle!I23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I23,IF(modèle!I23 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F22" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J22) &gt; 0, modèle!J22,""),IF(LEN(modèle!K22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K22,IF(modèle!K22 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J23) &gt; 0, modèle!J23,""),IF(LEN(modèle!K23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K23,IF(modèle!K23 &gt; 1," points"," point")),""))</f>
         <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
-        <f>IF(LEN(modèle!A23) &gt; 0, modèle!A23,"")</f>
+        <f>IF(LEN(modèle!A24) &gt; 0, modèle!A24,"")</f>
         <v>Internationalisation</v>
       </c>
       <c r="B23" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B23) &gt; 0, modèle!B23,""),IF(LEN(modèle!C23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C23,IF(modèle!C23 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B24) &gt; 0, modèle!B24,""),IF(LEN(modèle!C24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C24,IF(modèle!C24 &gt; 1," points"," point")),""))</f>
         <v>L’application est entièrement internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D23) &gt; 0, modèle!D23,""),IF(LEN(modèle!E23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E23,IF(modèle!E23 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D24) &gt; 0, modèle!D24,""),IF(LEN(modèle!E24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E24,IF(modèle!E24 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D23" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F23) &gt; 0, modèle!F23,""),IF(LEN(modèle!G23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G23,IF(modèle!G23 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F24) &gt; 0, modèle!F24,""),IF(LEN(modèle!G24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G24,IF(modèle!G24 &gt; 1," points"," point")),""))</f>
         <v>L’application est partiellement internationaliséeen Français et en Anglais&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E23" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H23) &gt; 0, modèle!H23,""),IF(LEN(modèle!I23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I23,IF(modèle!I23 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H24) &gt; 0, modèle!H24,""),IF(LEN(modèle!I24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I24,IF(modèle!I24 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F23" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J23) &gt; 0, modèle!J23,""),IF(LEN(modèle!K23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K23,IF(modèle!K23 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J24) &gt; 0, modèle!J24,""),IF(LEN(modèle!K24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K24,IF(modèle!K24 &gt; 1," points"," point")),""))</f>
         <v>L’application n’est pas internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
-        <f>IF(LEN(modèle!A24) &gt; 0, modèle!A24,"")</f>
+        <f>IF(LEN(modèle!A25) &gt; 0, modèle!A25,"")</f>
         <v>Organisation visuelle</v>
       </c>
       <c r="B24" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B24) &gt; 0, modèle!B24,""),IF(LEN(modèle!C24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C24,IF(modèle!C24 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B25) &gt; 0, modèle!B25,""),IF(LEN(modèle!C25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C25,IF(modèle!C25 &gt; 1," points"," point")),""))</f>
         <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D24) &gt; 0, modèle!D24,""),IF(LEN(modèle!E24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E24,IF(modèle!E24 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D25) &gt; 0, modèle!D25,""),IF(LEN(modèle!E25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E25,IF(modèle!E25 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D24" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F24) &gt; 0, modèle!F24,""),IF(LEN(modèle!G24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G24,IF(modèle!G24 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F25) &gt; 0, modèle!F25,""),IF(LEN(modèle!G25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G25,IF(modèle!G25 &gt; 1," points"," point")),""))</f>
         <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H24) &gt; 0, modèle!H24,""),IF(LEN(modèle!I24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I24,IF(modèle!I24 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H25) &gt; 0, modèle!H25,""),IF(LEN(modèle!I25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I25,IF(modèle!I25 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F24" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J24) &gt; 0, modèle!J24,""),IF(LEN(modèle!K24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K24,IF(modèle!K24 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J25) &gt; 0, modèle!J25,""),IF(LEN(modèle!K25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K25,IF(modèle!K25 &gt; 1," points"," point")),""))</f>
         <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
-        <f>IF(LEN(modèle!A25) &gt; 0, modèle!A25,"")</f>
+        <f>IF(LEN(modèle!A26) &gt; 0, modèle!A26,"")</f>
         <v>Navigation</v>
       </c>
       <c r="B25" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B25) &gt; 0, modèle!B25,""),IF(LEN(modèle!C25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C25,IF(modèle!C25 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B26) &gt; 0, modèle!B26,""),IF(LEN(modèle!C26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C26,IF(modèle!C26 &gt; 1," points"," point")),""))</f>
         <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D25) &gt; 0, modèle!D25,""),IF(LEN(modèle!E25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E25,IF(modèle!E25 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D26) &gt; 0, modèle!D26,""),IF(LEN(modèle!E26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E26,IF(modèle!E26 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D25" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F25) &gt; 0, modèle!F25,""),IF(LEN(modèle!G25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G25,IF(modèle!G25 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F26) &gt; 0, modèle!F26,""),IF(LEN(modèle!G26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G26,IF(modèle!G26 &gt; 1," points"," point")),""))</f>
         <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H25) &gt; 0, modèle!H25,""),IF(LEN(modèle!I25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I25,IF(modèle!I25 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H26) &gt; 0, modèle!H26,""),IF(LEN(modèle!I26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I26,IF(modèle!I26 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F25" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J25) &gt; 0, modèle!J25,""),IF(LEN(modèle!K25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K25,IF(modèle!K25 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J26) &gt; 0, modèle!J26,""),IF(LEN(modèle!K26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K26,IF(modèle!K26 &gt; 1," points"," point")),""))</f>
         <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="str">
-        <f>IF(LEN(modèle!A26) &gt; 0, modèle!A26,"")</f>
+        <f>IF(LEN(modèle!A27) &gt; 0, modèle!A27,"")</f>
         <v>PWA</v>
       </c>
       <c r="B26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B26) &gt; 0, modèle!B26,""),IF(LEN(modèle!C26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C26,IF(modèle!C26 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B27) &gt; 0, modèle!B27,""),IF(LEN(modèle!C27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C27,IF(modèle!C27 &gt; 1," points"," point")),""))</f>
         <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 75% des exigences.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D26) &gt; 0, modèle!D26,""),IF(LEN(modèle!E26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E26,IF(modèle!E26 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D27) &gt; 0, modèle!D27,""),IF(LEN(modèle!E27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E27,IF(modèle!E27 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F26) &gt; 0, modèle!F26,""),IF(LEN(modèle!G26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G26,IF(modèle!G26 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F27) &gt; 0, modèle!F27,""),IF(LEN(modèle!G27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G27,IF(modèle!G27 &gt; 1," points"," point")),""))</f>
         <v>L’application est configurée en tant qu’application progressive (PWA) et répond à plus de 50% des exigences.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H26) &gt; 0, modèle!H26,""),IF(LEN(modèle!I26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I26,IF(modèle!I26 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H27) &gt; 0, modèle!H27,""),IF(LEN(modèle!I27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I27,IF(modèle!I27 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J26) &gt; 0, modèle!J26,""),IF(LEN(modèle!K26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K26,IF(modèle!K26 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J27) &gt; 0, modèle!J27,""),IF(LEN(modèle!K27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K27,IF(modèle!K27 &gt; 1," points"," point")),""))</f>
         <v>L’application est configurée en tant qu’application progressive (PWA) ou répond à moins de 50% des exigences.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="str">
-        <f>IF(LEN(modèle!A27) &gt; 0, modèle!A27,"")</f>
+        <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
         <v>Publication</v>
       </c>
       <c r="B27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B27) &gt; 0, modèle!B27,""),IF(LEN(modèle!C27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C27,IF(modèle!C27 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
         <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D27) &gt; 0, modèle!D27,""),IF(LEN(modèle!E27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E27,IF(modèle!E27 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F27) &gt; 0, modèle!F27,""),IF(LEN(modèle!G27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G27,IF(modèle!G27 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
         <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H27) &gt; 0, modèle!H27,""),IF(LEN(modèle!I27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I27,IF(modèle!I27 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J27) &gt; 0, modèle!J27,""),IF(LEN(modèle!K27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K27,IF(modèle!K27 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
         <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="str">
-        <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
+        <f>IF(LEN(modèle!A29) &gt; 0, modèle!A29,"")</f>
         <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B28" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B29) &gt; 0, modèle!B29,""),IF(LEN(modèle!C29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C29,IF(modèle!C29 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D29) &gt; 0, modèle!D29,""),IF(LEN(modèle!E29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E29,IF(modèle!E29 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="D28" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F29) &gt; 0, modèle!F29,""),IF(LEN(modèle!G29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G29,IF(modèle!G29 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="E28" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H29) &gt; 0, modèle!H29,""),IF(LEN(modèle!I29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I29,IF(modèle!I29 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
       <c r="F28" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J29) &gt; 0, modèle!J29,""),IF(LEN(modèle!K29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K29,IF(modèle!K29 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
@@ -1442,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004F3CC3-38A6-1349-9E0D-D575CD7A9164}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1508,7 +1526,7 @@
         <v>9</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
@@ -1517,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M18" si="0">MAX(C3,E3,G3,I3)</f>
+        <f t="shared" ref="M3:M19" si="0">MAX(C3,E3,G3,I3)</f>
         <v>6</v>
       </c>
     </row>
@@ -1586,25 +1604,25 @@
         <v>91</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>93</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>95</v>
@@ -1614,7 +1632,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1712,13 +1730,13 @@
         <v>32</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
@@ -1728,7 +1746,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1739,13 +1757,13 @@
         <v>37</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" t="s">
         <v>39</v>
@@ -1755,75 +1773,105 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
+      <c r="F14" t="s">
+        <v>41</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>47</v>
+      <c r="F15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>50</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
@@ -1832,61 +1880,37 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="H17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18">
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1898,88 +1922,94 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="G19">
-        <v>7</v>
-      </c>
-      <c r="H19" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" ref="M19:M27" si="1">MAX(C19,E19,G19,I19)</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20">
         <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" ref="M20:M28" si="1">MAX(C20,E20,G20,I20)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="G21">
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1989,132 +2019,132 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22">
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24">
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24">
         <v>3</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
       <c r="J24" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25">
+      <c r="F25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25">
         <v>2</v>
       </c>
-      <c r="F25" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
       <c r="J25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2126,22 +2156,22 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2151,8 +2181,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout IA dans projet intégrateur
</commit_message>
<xml_diff>
--- a/template/grille_correction.xlsx
+++ b/template/grille_correction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/developpementweb3/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7A2299-529C-5C40-839A-ADF43CDD37B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D22CB16-3775-8447-81F7-DDF62262EF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
   <si>
     <t>Élément</t>
   </si>
@@ -349,6 +349,18 @@
   </si>
   <si>
     <t>Les tests unitaires ne couvrent que __25%__ des méthodes HTTP et validations</t>
+  </si>
+  <si>
+    <t>Compréhension de son code</t>
+  </si>
+  <si>
+    <t>L'élève explique clairement et sans hésitation l'ensemble du code remis à l'enseignant</t>
+  </si>
+  <si>
+    <t>L'élève explique clairement et sans hésitation une majeure partie du code remis à l'enseignant</t>
+  </si>
+  <si>
+    <t>L'élève explique difficilement son code</t>
   </si>
 </sst>
 </file>
@@ -703,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,11 +1066,11 @@
     <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>IF(LEN(modèle!A15) &gt; 0, modèle!A15,"")</f>
-        <v>Documentation</v>
+        <v>Compréhension de son code</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B15) &gt; 0, modèle!B15,""),IF(LEN(modèle!C15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C15,IF(modèle!C15 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L'élève explique clairement et sans hésitation l'ensemble du code remis à l'enseignant&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D15) &gt; 0, modèle!D15,""),IF(LEN(modèle!E15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E15,IF(modèle!E15 &gt; 1," points"," point")),""))</f>
@@ -1066,7 +1078,7 @@
       </c>
       <c r="D14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F15) &gt; 0, modèle!F15,""),IF(LEN(modèle!G15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G15,IF(modèle!G15 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L'élève explique clairement et sans hésitation une majeure partie du code remis à l'enseignant&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H15) &gt; 0, modèle!H15,""),IF(LEN(modèle!I15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I15,IF(modèle!I15 &gt; 1," points"," point")),""))</f>
@@ -1074,17 +1086,17 @@
       </c>
       <c r="F14" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J15) &gt; 0, modèle!J15,""),IF(LEN(modèle!K15) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K15,IF(modèle!K15 &gt; 1," points"," point")),""))</f>
-        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>L'élève explique difficilement son code&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>IF(LEN(modèle!A16) &gt; 0, modèle!A16,"")</f>
-        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
+        <v>Documentation</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B16) &gt; 0, modèle!B16,""),IF(LEN(modèle!C16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C16,IF(modèle!C16 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>La documentation de l’interface applicative est claire et complète. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D16) &gt; 0, modèle!D16,""),IF(LEN(modèle!E16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E16,IF(modèle!E16 &gt; 1," points"," point")),""))</f>
@@ -1092,7 +1104,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F16) &gt; 0, modèle!F16,""),IF(LEN(modèle!G16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G16,IF(modèle!G16 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>La documentation de l’interface applicative est floue ou incomplète.&lt;br/&gt;&lt;br/&gt;1 point</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H16) &gt; 0, modèle!H16,""),IF(LEN(modèle!I16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I16,IF(modèle!I16 &gt; 1," points"," point")),""))</f>
@@ -1100,13 +1112,13 @@
       </c>
       <c r="F15" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J16) &gt; 0, modèle!J16,""),IF(LEN(modèle!K16) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K16,IF(modèle!K16 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>La documentation de l’interface applicative est inexistante.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f>IF(LEN(modèle!A17) &gt; 0, modèle!A17,"")</f>
-        <v>__Application Web (50%)__ {: colspan=5}</v>
+        <v>La qualité générale de l’interface applicative (API) démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B17) &gt; 0, modèle!B17,""),IF(LEN(modèle!C17) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C17,IF(modèle!C17 &gt; 1," points"," point")),""))</f>
@@ -1129,14 +1141,14 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>IF(LEN(modèle!A18) &gt; 0, modèle!A18,"")</f>
-        <v>Composants</v>
+        <v>__Application Web (50%)__ {: colspan=5}</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B18) &gt; 0, modèle!B18,""),IF(LEN(modèle!C18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C18,IF(modèle!C18 &gt; 1," points"," point")),""))</f>
-        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D18) &gt; 0, modèle!D18,""),IF(LEN(modèle!E18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E18,IF(modèle!E18 &gt; 1," points"," point")),""))</f>
@@ -1144,103 +1156,103 @@
       </c>
       <c r="D17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F18) &gt; 0, modèle!F18,""),IF(LEN(modèle!G18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G18,IF(modèle!G18 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v/>
       </c>
       <c r="E17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H18) &gt; 0, modèle!H18,""),IF(LEN(modèle!I18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I18,IF(modèle!I18 &gt; 1," points"," point")),""))</f>
-        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v/>
       </c>
       <c r="F17" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J18) &gt; 0, modèle!J18,""),IF(LEN(modèle!K18) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K18,IF(modèle!K18 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>IF(LEN(modèle!A19) &gt; 0, modèle!A19,"")</f>
-        <v>Hooks</v>
+        <v>Composants</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B19) &gt; 0, modèle!B19,""),IF(LEN(modèle!C19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C19,IF(modèle!C19 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application est optimalement décomposée en composants.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D19) &gt; 0, modèle!D19,""),IF(LEN(modèle!E19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E19,IF(modèle!E19 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="D18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F19) &gt; 0, modèle!F19,""),IF(LEN(modèle!G19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G19,IF(modèle!G19 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est correctement décomposée en composants&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H19) &gt; 0, modèle!H19,""),IF(LEN(modèle!I19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I19,IF(modèle!I19 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application est décomposée en composants, mais contient une ou 2 erreurs de structure. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="F18" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J19) &gt; 0, modèle!J19,""),IF(LEN(modèle!K19) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K19,IF(modèle!K19 &gt; 1," points"," point")),""))</f>
-        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas correctement décomposée&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>IF(LEN(modèle!A20) &gt; 0, modèle!A20,"")</f>
-        <v>Méthodes HTTP</v>
+        <v>Hooks</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B20) &gt; 0, modèle!B20,""),IF(LEN(modèle!C20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C20,IF(modèle!C20 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
+        <v>Les techniques de programmation utilisées démontrent une excellente maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D20) &gt; 0, modèle!D20,""),IF(LEN(modèle!E20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E20,IF(modèle!E20 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
+        <v>Les techniques de programmation utilisées démontrent une bonne maîtrise de l’approche par hooks &lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="D19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F20) &gt; 0, modèle!F20,""),IF(LEN(modèle!G20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G20,IF(modèle!G20 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
+        <v>Les techniques de programmation utilisées démontrent une légère maîtrise de l’approche par hooks&lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H20) &gt; 0, modèle!H20,""),IF(LEN(modèle!I20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I20,IF(modèle!I20 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v/>
       </c>
       <c r="F19" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J20) &gt; 0, modèle!J20,""),IF(LEN(modèle!K20) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K20,IF(modèle!K20 &gt; 1," points"," point")),""))</f>
-        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>Les techniques de programmation utilisées ne démontrent pas la maîtrise de l’approchepar hooks&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>IF(LEN(modèle!A21) &gt; 0, modèle!A21,"")</f>
-        <v>Validations</v>
+        <v>Méthodes HTTP</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B21) &gt; 0, modèle!B21,""),IF(LEN(modèle!C21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C21,IF(modèle!C21 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations appropriées avec messages à l'utilisateur dans l'interface graphique.&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application implémente correctement l’ensemble des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;12 points</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D21) &gt; 0, modèle!D21,""),IF(LEN(modèle!E21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E21,IF(modèle!E21 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application implémente correctement 75% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;9 points</v>
       </c>
       <c r="D20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F21) &gt; 0, modèle!F21,""),IF(LEN(modèle!G21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G21,IF(modèle!G21 &gt; 1," points"," point")),""))</f>
-        <v>L’application contient des validations partiellement appropriées qui ont des messages affichés à l'utilisateur.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application implémente correctement 50% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;7 points</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H21) &gt; 0, modèle!H21,""),IF(LEN(modèle!I21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I21,IF(modèle!I21 &gt; 1," points"," point")),""))</f>
-        <v/>
+        <v>L’application implémente correctement 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="F20" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J21) &gt; 0, modèle!J21,""),IF(LEN(modèle!K21) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K21,IF(modèle!K21 &gt; 1," points"," point")),""))</f>
-        <v>L’application ne contient pas de validations appropriées ou ne sont pas affichées à l'utilisateur.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>L’application implémente correctement moins de 25% des méthodes HTTP fournies par l’interface applicative (API).&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>IF(LEN(modèle!A22) &gt; 0, modèle!A22,"")</f>
-        <v>Visuel</v>
+        <v>Validations</v>
       </c>
       <c r="B21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B22) &gt; 0, modèle!B22,""),IF(LEN(modèle!C22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C22,IF(modèle!C22 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application contient des validations appropriées avec messages à l'utilisateur dans l'interface graphique.&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D22) &gt; 0, modèle!D22,""),IF(LEN(modèle!E22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E22,IF(modèle!E22 &gt; 1," points"," point")),""))</f>
@@ -1248,7 +1260,7 @@
       </c>
       <c r="D21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F22) &gt; 0, modèle!F22,""),IF(LEN(modèle!G22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G22,IF(modèle!G22 &gt; 1," points"," point")),""))</f>
-        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application contient des validations partiellement appropriées qui ont des messages affichés à l'utilisateur.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H22) &gt; 0, modèle!H22,""),IF(LEN(modèle!I22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I22,IF(modèle!I22 &gt; 1," points"," point")),""))</f>
@@ -1256,17 +1268,17 @@
       </c>
       <c r="F21" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J22) &gt; 0, modèle!J22,""),IF(LEN(modèle!K22) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K22,IF(modèle!K22 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>L’application ne contient pas de validations appropriées ou ne sont pas affichées à l'utilisateur.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="str">
         <f>IF(LEN(modèle!A23) &gt; 0, modèle!A23,"")</f>
-        <v>Application sécurisée</v>
+        <v>Compréhension de son code</v>
       </c>
       <c r="B22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B23) &gt; 0, modèle!B23,""),IF(LEN(modèle!C23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C23,IF(modèle!C23 &gt; 1," points"," point")),""))</f>
-        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
+        <v>L'élève explique clairement et sans hésitation l'ensemble du code remis à l'enseignant&lt;br/&gt;&lt;br/&gt;5 points</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D23) &gt; 0, modèle!D23,""),IF(LEN(modèle!E23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E23,IF(modèle!E23 &gt; 1," points"," point")),""))</f>
@@ -1274,7 +1286,7 @@
       </c>
       <c r="D22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F23) &gt; 0, modèle!F23,""),IF(LEN(modèle!G23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G23,IF(modèle!G23 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L'élève explique clairement et sans hésitation une majeure partie du code remis à l'enseignant&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H23) &gt; 0, modèle!H23,""),IF(LEN(modèle!I23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I23,IF(modèle!I23 &gt; 1," points"," point")),""))</f>
@@ -1282,17 +1294,17 @@
       </c>
       <c r="F22" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J23) &gt; 0, modèle!J23,""),IF(LEN(modèle!K23) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K23,IF(modèle!K23 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
+        <v>L'élève explique difficilement son code&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>IF(LEN(modèle!A24) &gt; 0, modèle!A24,"")</f>
-        <v>Internationalisation</v>
+        <v>Visuel</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B24) &gt; 0, modèle!B24,""),IF(LEN(modèle!C24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C24,IF(modèle!C24 &gt; 1," points"," point")),""))</f>
-        <v>L’application est entièrement internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;5 points</v>
+        <v>L’application intègre adéquatement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D24) &gt; 0, modèle!D24,""),IF(LEN(modèle!E24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E24,IF(modèle!E24 &gt; 1," points"," point")),""))</f>
@@ -1300,7 +1312,7 @@
       </c>
       <c r="D23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F24) &gt; 0, modèle!F24,""),IF(LEN(modèle!G24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G24,IF(modèle!G24 &gt; 1," points"," point")),""))</f>
-        <v>L’application est partiellement internationaliséeen Français et en Anglais&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application intègre partiellement des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;2 points</v>
       </c>
       <c r="E23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H24) &gt; 0, modèle!H24,""),IF(LEN(modèle!I24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I24,IF(modèle!I24 &gt; 1," points"," point")),""))</f>
@@ -1308,17 +1320,17 @@
       </c>
       <c r="F23" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J24) &gt; 0, modèle!J24,""),IF(LEN(modèle!K24) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K24,IF(modèle!K24 &gt; 1," points"," point")),""))</f>
-        <v>L’application n’est pas internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’application n’intègre pas des composants visuels répondant aux exigences du projet. &lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="str">
         <f>IF(LEN(modèle!A25) &gt; 0, modèle!A25,"")</f>
-        <v>Organisation visuelle</v>
+        <v>Application sécurisée</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B25) &gt; 0, modèle!B25,""),IF(LEN(modèle!C25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C25,IF(modèle!C25 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est correctement sécurisée.&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D25) &gt; 0, modèle!D25,""),IF(LEN(modèle!E25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E25,IF(modèle!E25 &gt; 1," points"," point")),""))</f>
@@ -1326,7 +1338,7 @@
       </c>
       <c r="D24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F25) &gt; 0, modèle!F25,""),IF(LEN(modèle!G25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G25,IF(modèle!G25 &gt; 1," points"," point")),""))</f>
-        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est partiellement sécurisée.&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H25) &gt; 0, modèle!H25,""),IF(LEN(modèle!I25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I25,IF(modèle!I25 &gt; 1," points"," point")),""))</f>
@@ -1334,17 +1346,17 @@
       </c>
       <c r="F24" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J25) &gt; 0, modèle!J25,""),IF(LEN(modèle!K25) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K25,IF(modèle!K25 &gt; 1," points"," point")),""))</f>
-        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>L’application n’est pas sécurisée.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="str">
         <f>IF(LEN(modèle!A26) &gt; 0, modèle!A26,"")</f>
-        <v>Navigation</v>
+        <v>Internationalisation</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!B26) &gt; 0, modèle!B26,""),IF(LEN(modèle!C26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C26,IF(modèle!C26 &gt; 1," points"," point")),""))</f>
-        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;3 points</v>
+        <v>L’application est entièrement internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;4 points</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!D26) &gt; 0, modèle!D26,""),IF(LEN(modèle!E26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E26,IF(modèle!E26 &gt; 1," points"," point")),""))</f>
@@ -1352,7 +1364,7 @@
       </c>
       <c r="D25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!F26) &gt; 0, modèle!F26,""),IF(LEN(modèle!G26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G26,IF(modèle!G26 &gt; 1," points"," point")),""))</f>
-        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;2 points</v>
+        <v>L’application est partiellement internationaliséeen Français et en Anglais&lt;br/&gt;&lt;br/&gt;3 points</v>
       </c>
       <c r="E25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!H26) &gt; 0, modèle!H26,""),IF(LEN(modèle!I26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I26,IF(modèle!I26 &gt; 1," points"," point")),""))</f>
@@ -1360,58 +1372,110 @@
       </c>
       <c r="F25" s="1" t="str">
         <f>_xlfn.CONCAT(IF(LEN(modèle!J26) &gt; 0, modèle!J26,""),IF(LEN(modèle!K26) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K26,IF(modèle!K26 &gt; 1," points"," point")),""))</f>
+        <v>L’application n’est pas internationalisée en Français et en Anglais&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="str">
+        <f>IF(LEN(modèle!A27) &gt; 0, modèle!A27,"")</f>
+        <v>Organisation visuelle</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B27) &gt; 0, modèle!B27,""),IF(LEN(modèle!C27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C27,IF(modèle!C27 &gt; 1," points"," point")),""))</f>
+        <v>L’organisation visuelle des fonctionnalités est adéquate et cohérente dans un minimum de 3 affichages (mobile, tablette et PC)&lt;br/&gt;&lt;br/&gt;2 points</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D27) &gt; 0, modèle!D27,""),IF(LEN(modèle!E27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E27,IF(modèle!E27 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F27) &gt; 0, modèle!F27,""),IF(LEN(modèle!G27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G27,IF(modèle!G27 &gt; 1," points"," point")),""))</f>
+        <v>Les fonctionnalités développées contiennent 1 ou 2 incohérences au niveau de l’organisation visuelle.&lt;br/&gt;&lt;br/&gt;1 point</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H27) &gt; 0, modèle!H27,""),IF(LEN(modèle!I27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I27,IF(modèle!I27 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J27) &gt; 0, modèle!J27,""),IF(LEN(modèle!K27) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K27,IF(modèle!K27 &gt; 1," points"," point")),""))</f>
+        <v>L’organisation visuelle des fonctionnalités développées est inadéquate ou incohérente.&lt;br/&gt;&lt;br/&gt;0 point</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="str">
+        <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
+        <v>Navigation</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
+        <v>La navigation est intuitive.&lt;br/&gt;_(Positionnement des boutons, retour à l’accueil, utilisation d’onglets, etc.)_&lt;br/&gt;&lt;br/&gt;2 points</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
+        <v>La navigation contient une erreur de parcours.&lt;br/&gt;&lt;br/&gt;1 point</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
         <v>La navigation contient plus d’une erreur de parcours.&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
-        <f>IF(LEN(modèle!A28) &gt; 0, modèle!A28,"")</f>
+    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="str">
+        <f>IF(LEN(modèle!A30) &gt; 0, modèle!A30,"")</f>
         <v>Publication</v>
       </c>
-      <c r="B26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B28) &gt; 0, modèle!B28,""),IF(LEN(modèle!C28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C28,IF(modèle!C28 &gt; 1," points"," point")),""))</f>
-        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;3 points</v>
-      </c>
-      <c r="C26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D28) &gt; 0, modèle!D28,""),IF(LEN(modèle!E28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E28,IF(modèle!E28 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="D26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F28) &gt; 0, modèle!F28,""),IF(LEN(modèle!G28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G28,IF(modèle!G28 &gt; 1," points"," point")),""))</f>
-        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;2 points</v>
-      </c>
-      <c r="E26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H28) &gt; 0, modèle!H28,""),IF(LEN(modèle!I28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I28,IF(modèle!I28 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="F26" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J28) &gt; 0, modèle!J28,""),IF(LEN(modèle!K28) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K28,IF(modèle!K28 &gt; 1," points"," point")),""))</f>
+      <c r="B28" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B30) &gt; 0, modèle!B30,""),IF(LEN(modèle!C30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C30,IF(modèle!C30 &gt; 1," points"," point")),""))</f>
+        <v>L’application est publiée et fonctionnelle.&lt;br/&gt;&lt;br/&gt;2 points</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D30) &gt; 0, modèle!D30,""),IF(LEN(modèle!E30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E30,IF(modèle!E30 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F30) &gt; 0, modèle!F30,""),IF(LEN(modèle!G30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G30,IF(modèle!G30 &gt; 1," points"," point")),""))</f>
+        <v>L’interface applicative n’est pas correctement publiée.  Certaines fonctionnalités ne fonctionnement pas. &lt;br/&gt;&lt;br/&gt;1 point</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H30) &gt; 0, modèle!H30,""),IF(LEN(modèle!I30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I30,IF(modèle!I30 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J30) &gt; 0, modèle!J30,""),IF(LEN(modèle!K30) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K30,IF(modèle!K30 &gt; 1," points"," point")),""))</f>
         <v>L’application n’est pas publiée&lt;br/&gt;&lt;br/&gt;0 point</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="str">
-        <f>IF(LEN(modèle!A29) &gt; 0, modèle!A29,"")</f>
+    <row r="29" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="str">
+        <f>IF(LEN(modèle!A31) &gt; 0, modèle!A31,"")</f>
         <v>La qualité générale de l’application démontre une rigueur dans l’application des procédures d’assurance qualité.&lt;br/&gt;{==(Correction négative, -1 par bogue identifié)==} {: colspan=5}</v>
       </c>
-      <c r="B27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!B29) &gt; 0, modèle!B29,""),IF(LEN(modèle!C29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C29,IF(modèle!C29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="C27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!D29) &gt; 0, modèle!D29,""),IF(LEN(modèle!E29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E29,IF(modèle!E29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!F29) &gt; 0, modèle!F29,""),IF(LEN(modèle!G29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G29,IF(modèle!G29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="E27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!H29) &gt; 0, modèle!H29,""),IF(LEN(modèle!I29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I29,IF(modèle!I29 &gt; 1," points"," point")),""))</f>
-        <v/>
-      </c>
-      <c r="F27" s="1" t="str">
-        <f>_xlfn.CONCAT(IF(LEN(modèle!J29) &gt; 0, modèle!J29,""),IF(LEN(modèle!K29) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K29,IF(modèle!K29 &gt; 1," points"," point")),""))</f>
+      <c r="B29" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!B31) &gt; 0, modèle!B31,""),IF(LEN(modèle!C31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!C31,IF(modèle!C31 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!D31) &gt; 0, modèle!D31,""),IF(LEN(modèle!E31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!E31,IF(modèle!E31 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="D29" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!F31) &gt; 0, modèle!F31,""),IF(LEN(modèle!G31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!G31,IF(modèle!G31 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!H31) &gt; 0, modèle!H31,""),IF(LEN(modèle!I31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!I31,IF(modèle!I31 &gt; 1," points"," point")),""))</f>
+        <v/>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f>_xlfn.CONCAT(IF(LEN(modèle!J31) &gt; 0, modèle!J31,""),IF(LEN(modèle!K31) &gt; 0,_xlfn.CONCAT("&lt;br/&gt;&lt;br/&gt;",modèle!K31,IF(modèle!K31 &gt; 1," points"," point")),""))</f>
         <v/>
       </c>
     </row>
@@ -1422,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004F3CC3-38A6-1349-9E0D-D575CD7A9164}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1497,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M19" si="0">MAX(C3,E3,G3,I3)</f>
+        <f t="shared" ref="M3:M20" si="0">MAX(C3,E3,G3,I3)</f>
         <v>6</v>
       </c>
     </row>
@@ -1804,45 +1868,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15" si="1">MAX(C15,E15,G15,I15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
         <v>45</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="136" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>47</v>
+      <c r="K16">
+        <v>0</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
@@ -1851,61 +1933,37 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18" t="s">
-        <v>55</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19">
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1917,240 +1975,300 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="G20">
-        <v>7</v>
-      </c>
-      <c r="H20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M28" si="1">MAX(C20,E20,G20,I20)</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21">
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21">
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" ref="M21:M30" si="2">MAX(C21,E21,G21,I21)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="G22">
         <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="J24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25">
         <v>3</v>
       </c>
-      <c r="J24" t="s">
-        <v>93</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
       <c r="J25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26">
         <v>3</v>
       </c>
-      <c r="F26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
       <c r="J26" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
       <c r="M27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
         <v>78</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
         <v>79</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>